<commit_message>
update java core sheet
</commit_message>
<xml_diff>
--- a/Training_Plan.xlsx
+++ b/Training_Plan.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="45" windowWidth="19155" windowHeight="11760" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="45" windowWidth="19155" windowHeight="8400" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Plan" sheetId="1" r:id="rId1"/>
@@ -14,6 +14,7 @@
     <sheet name="Spring framework" sheetId="5" r:id="rId5"/>
     <sheet name="MongoDBJasper" sheetId="6" r:id="rId6"/>
     <sheet name="JUNIT" sheetId="7" r:id="rId7"/>
+    <sheet name="Logging" sheetId="8" r:id="rId8"/>
   </sheets>
   <definedNames>
     <definedName name="jaxrs_intro" localSheetId="3">'RESTful WS'!$B$6</definedName>
@@ -23,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="583" uniqueCount="534">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="589" uniqueCount="538">
   <si>
     <t>Java core</t>
   </si>
@@ -9970,12 +9971,157 @@
       <t>);</t>
     </r>
   </si>
+  <si>
+    <t>1. What is logback?</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF333333"/>
+        <rFont val="Wingdings"/>
+        <charset val="2"/>
+      </rPr>
+      <t>Ø</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color rgb="FF333333"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+      </rPr>
+      <t>Logback</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF333333"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+      </rPr>
+      <t> is intended as a successor to the popular </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color rgb="FF333333"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+      </rPr>
+      <t>log4j</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF333333"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> project. 
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF333333"/>
+        <rFont val="Wingdings"/>
+        <charset val="2"/>
+      </rPr>
+      <t>Ø</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF333333"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">It builds upon a decade of experience gained in designing industrial-strength logging systems. 
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF333333"/>
+        <rFont val="Wingdings"/>
+        <charset val="2"/>
+      </rPr>
+      <t>Ø</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF333333"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+      </rPr>
+      <t>The resulting product, i.e. </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color rgb="FF333333"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+      </rPr>
+      <t>logback</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF333333"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">, is faster and has a smaller footprint than all existing logging systems, sometimes by a wide margin. 
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF333333"/>
+        <rFont val="Wingdings"/>
+        <charset val="2"/>
+      </rPr>
+      <t>Ø</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF333333"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+      </rPr>
+      <t>Just as importantly, logback offers unique and rather useful features missing in other logging systems.</t>
+    </r>
+  </si>
+  <si>
+    <t>What is SLF4J?</t>
+  </si>
+  <si>
+    <r>
+      <t>SLF4J</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF333333"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+      </rPr>
+      <t> is a simple facade for logging systems allowing the end-user to plug-in the desired logging system at deployment time.</t>
+    </r>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="45">
+  <fonts count="50">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -10286,6 +10432,35 @@
       <name val="Consolas"/>
       <family val="3"/>
     </font>
+    <font>
+      <sz val="23"/>
+      <color rgb="FF333333"/>
+      <name val="Helvetica"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF333333"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF333333"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF333333"/>
+      <name val="Wingdings"/>
+      <charset val="2"/>
+    </font>
+    <font>
+      <sz val="18"/>
+      <color rgb="FF333333"/>
+      <name val="Helvetica"/>
+    </font>
   </fonts>
   <fills count="5">
     <fill>
@@ -10481,7 +10656,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="109">
+  <cellXfs count="112">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -10699,6 +10874,24 @@
     <xf numFmtId="0" fontId="33" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="35" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="37" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="40" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="36" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="41" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="38" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="42" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
@@ -10729,24 +10922,15 @@
     <xf numFmtId="0" fontId="20" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="34" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="35" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="37" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1" readingOrder="1"/>
+    <xf numFmtId="0" fontId="45" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="40" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1" readingOrder="1"/>
+    <xf numFmtId="0" fontId="46" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="36" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1" readingOrder="1"/>
+    <xf numFmtId="0" fontId="49" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="41" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="38" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="42" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -10768,13 +10952,13 @@
     <xdr:from>
       <xdr:col>4</xdr:col>
       <xdr:colOff>47624</xdr:colOff>
-      <xdr:row>102</xdr:row>
+      <xdr:row>89</xdr:row>
       <xdr:rowOff>28575</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
       <xdr:colOff>85724</xdr:colOff>
-      <xdr:row>112</xdr:row>
+      <xdr:row>99</xdr:row>
       <xdr:rowOff>95250</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -10812,13 +10996,13 @@
     <xdr:from>
       <xdr:col>2</xdr:col>
       <xdr:colOff>752475</xdr:colOff>
-      <xdr:row>154</xdr:row>
+      <xdr:row>141</xdr:row>
       <xdr:rowOff>76200</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
       <xdr:colOff>3019425</xdr:colOff>
-      <xdr:row>193</xdr:row>
+      <xdr:row>180</xdr:row>
       <xdr:rowOff>114300</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -11658,10 +11842,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B2:E163"/>
+  <dimension ref="B2:E197"/>
   <sheetViews>
-    <sheetView topLeftCell="A102" workbookViewId="0">
-      <selection activeCell="D117" sqref="D117"/>
+    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="D51" sqref="D51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -11753,1343 +11937,1343 @@
     </row>
     <row r="10" spans="2:5" ht="31.5">
       <c r="B10" s="22" t="s">
-        <v>203</v>
+        <v>101</v>
       </c>
       <c r="C10" s="23"/>
       <c r="D10" s="23"/>
       <c r="E10" s="24"/>
     </row>
-    <row r="11" spans="2:5">
-      <c r="B11" s="19" t="s">
+    <row r="12" spans="2:5">
+      <c r="B12" s="19" t="s">
         <v>3</v>
       </c>
-      <c r="C11" s="19"/>
-      <c r="D11" s="19" t="s">
-        <v>35</v>
-      </c>
-      <c r="E11" s="19" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="12" spans="2:5" ht="165">
-      <c r="B12" s="2"/>
-      <c r="C12" s="2"/>
-      <c r="D12" s="10" t="s">
-        <v>204</v>
-      </c>
-      <c r="E12" s="29" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="13" spans="2:5">
-      <c r="B13" s="2"/>
-      <c r="C13" s="2"/>
-      <c r="D13" s="31" t="s">
-        <v>206</v>
-      </c>
-      <c r="E13" s="31" t="s">
-        <v>207</v>
-      </c>
+      <c r="C12" s="19"/>
+      <c r="D12" s="19" t="s">
+        <v>46</v>
+      </c>
+      <c r="E12" s="19" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="13" spans="2:5" ht="18.75">
+      <c r="B13" s="2">
+        <v>1</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D13" s="18" t="s">
+        <v>58</v>
+      </c>
+      <c r="E13" s="2"/>
     </row>
     <row r="14" spans="2:5">
       <c r="B14" s="2"/>
       <c r="C14" s="2"/>
-      <c r="D14" s="2" t="s">
-        <v>208</v>
-      </c>
-      <c r="E14" s="29" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="15" spans="2:5" ht="30">
+      <c r="D14" s="99" t="s">
+        <v>47</v>
+      </c>
+      <c r="E14" s="100"/>
+    </row>
+    <row r="15" spans="2:5">
       <c r="B15" s="2"/>
       <c r="C15" s="2"/>
-      <c r="D15" s="2" t="s">
-        <v>210</v>
-      </c>
-      <c r="E15" s="29" t="s">
-        <v>211</v>
+      <c r="D15" s="15" t="s">
+        <v>48</v>
+      </c>
+      <c r="E15" s="15" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="16" spans="2:5">
       <c r="B16" s="2"/>
       <c r="C16" s="2"/>
-      <c r="D16" s="2" t="s">
-        <v>212</v>
-      </c>
-      <c r="E16" s="29" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="17" spans="2:5">
+      <c r="D16" s="16" t="s">
+        <v>50</v>
+      </c>
+      <c r="E16" s="16" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="17" spans="2:5" ht="45">
       <c r="B17" s="2"/>
       <c r="C17" s="2"/>
-      <c r="D17" s="2" t="s">
-        <v>214</v>
-      </c>
-      <c r="E17" s="29" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="18" spans="2:5">
+      <c r="D17" s="16" t="s">
+        <v>52</v>
+      </c>
+      <c r="E17" s="16" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="18" spans="2:5" ht="30">
       <c r="B18" s="2"/>
       <c r="C18" s="2"/>
-      <c r="D18" s="2" t="s">
-        <v>216</v>
-      </c>
-      <c r="E18" s="29" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="19" spans="2:5" ht="74.25" customHeight="1">
+      <c r="D18" s="16" t="s">
+        <v>54</v>
+      </c>
+      <c r="E18" s="16" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="19" spans="2:5">
       <c r="B19" s="2"/>
-      <c r="C19" s="32"/>
-      <c r="D19" s="33" t="s">
-        <v>218</v>
-      </c>
-      <c r="E19" s="30" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="20" spans="2:5" ht="78.75">
+      <c r="C19" s="2"/>
+      <c r="D19" s="16" t="s">
+        <v>56</v>
+      </c>
+      <c r="E19" s="16" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="20" spans="2:5" ht="18.75">
       <c r="B20" s="2"/>
-      <c r="C20" s="32"/>
-      <c r="D20" s="33" t="s">
-        <v>212</v>
-      </c>
-      <c r="E20" s="30" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="21" spans="2:5" ht="93.75">
+      <c r="C20" s="2"/>
+      <c r="D20" s="18" t="s">
+        <v>77</v>
+      </c>
+      <c r="E20" s="16"/>
+    </row>
+    <row r="21" spans="2:5">
       <c r="B21" s="2"/>
-      <c r="C21" s="32"/>
-      <c r="D21" s="1" t="s">
-        <v>221</v>
-      </c>
-      <c r="E21" s="30" t="s">
-        <v>222</v>
-      </c>
+      <c r="C21" s="2"/>
+      <c r="D21" s="103" t="s">
+        <v>78</v>
+      </c>
+      <c r="E21" s="103"/>
     </row>
     <row r="22" spans="2:5">
       <c r="B22" s="2"/>
       <c r="C22" s="2"/>
-      <c r="D22" s="2"/>
-      <c r="E22" s="29"/>
-    </row>
-    <row r="23" spans="2:5" ht="31.5">
-      <c r="B23" s="22" t="s">
-        <v>101</v>
-      </c>
-      <c r="C23" s="23"/>
-      <c r="D23" s="23"/>
-      <c r="E23" s="24"/>
-    </row>
-    <row r="25" spans="2:5">
-      <c r="B25" s="19" t="s">
-        <v>3</v>
-      </c>
-      <c r="C25" s="19"/>
-      <c r="D25" s="19" t="s">
-        <v>46</v>
-      </c>
-      <c r="E25" s="19" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="26" spans="2:5" ht="18.75">
-      <c r="B26" s="2">
-        <v>1</v>
-      </c>
-      <c r="C26" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="D26" s="18" t="s">
-        <v>58</v>
-      </c>
-      <c r="E26" s="2"/>
-    </row>
-    <row r="27" spans="2:5">
+      <c r="D22" s="15" t="s">
+        <v>48</v>
+      </c>
+      <c r="E22" s="15" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="23" spans="2:5">
+      <c r="B23" s="2"/>
+      <c r="C23" s="2"/>
+      <c r="D23" s="14" t="s">
+        <v>80</v>
+      </c>
+      <c r="E23" s="14" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="24" spans="2:5" ht="45">
+      <c r="B24" s="2"/>
+      <c r="C24" s="2"/>
+      <c r="D24" s="74" t="s">
+        <v>420</v>
+      </c>
+      <c r="E24" s="14" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="25" spans="2:5" ht="30">
+      <c r="B25" s="2"/>
+      <c r="C25" s="2"/>
+      <c r="D25" s="74" t="s">
+        <v>421</v>
+      </c>
+      <c r="E25" s="14" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="26" spans="2:5" ht="30">
+      <c r="B26" s="2"/>
+      <c r="C26" s="2"/>
+      <c r="D26" s="74" t="s">
+        <v>422</v>
+      </c>
+      <c r="E26" s="14" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="27" spans="2:5" ht="18.75">
       <c r="B27" s="2"/>
       <c r="C27" s="2"/>
-      <c r="D27" s="91" t="s">
-        <v>47</v>
-      </c>
-      <c r="E27" s="92"/>
+      <c r="D27" s="20" t="s">
+        <v>85</v>
+      </c>
+      <c r="E27" s="20"/>
     </row>
     <row r="28" spans="2:5">
       <c r="B28" s="2"/>
       <c r="C28" s="2"/>
-      <c r="D28" s="15" t="s">
-        <v>48</v>
-      </c>
-      <c r="E28" s="15" t="s">
-        <v>49</v>
-      </c>
+      <c r="D28" s="104" t="s">
+        <v>86</v>
+      </c>
+      <c r="E28" s="105"/>
     </row>
     <row r="29" spans="2:5">
       <c r="B29" s="2"/>
       <c r="C29" s="2"/>
-      <c r="D29" s="16" t="s">
-        <v>50</v>
-      </c>
-      <c r="E29" s="16" t="s">
-        <v>51</v>
+      <c r="D29" s="15" t="s">
+        <v>87</v>
+      </c>
+      <c r="E29" s="15" t="s">
+        <v>88</v>
       </c>
     </row>
     <row r="30" spans="2:5" ht="45">
       <c r="B30" s="2"/>
       <c r="C30" s="2"/>
-      <c r="D30" s="16" t="s">
-        <v>52</v>
-      </c>
-      <c r="E30" s="16" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="31" spans="2:5" ht="30">
+      <c r="D30" s="14" t="s">
+        <v>89</v>
+      </c>
+      <c r="E30" s="14" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="31" spans="2:5">
       <c r="B31" s="2"/>
       <c r="C31" s="2"/>
-      <c r="D31" s="16" t="s">
-        <v>54</v>
-      </c>
-      <c r="E31" s="16" t="s">
-        <v>55</v>
+      <c r="D31" s="14" t="s">
+        <v>91</v>
+      </c>
+      <c r="E31" s="14" t="s">
+        <v>92</v>
       </c>
     </row>
     <row r="32" spans="2:5">
       <c r="B32" s="2"/>
       <c r="C32" s="2"/>
-      <c r="D32" s="16" t="s">
-        <v>56</v>
-      </c>
-      <c r="E32" s="16" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="33" spans="2:5" ht="18.75">
+      <c r="D32" s="14" t="s">
+        <v>93</v>
+      </c>
+      <c r="E32" s="14" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="33" spans="2:5">
       <c r="B33" s="2"/>
       <c r="C33" s="2"/>
-      <c r="D33" s="18" t="s">
-        <v>77</v>
-      </c>
-      <c r="E33" s="16"/>
-    </row>
-    <row r="34" spans="2:5">
+      <c r="D33" s="14" t="s">
+        <v>95</v>
+      </c>
+      <c r="E33" s="14" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="34" spans="2:5" ht="30">
       <c r="B34" s="2"/>
       <c r="C34" s="2"/>
-      <c r="D34" s="95" t="s">
-        <v>78</v>
-      </c>
-      <c r="E34" s="95"/>
+      <c r="D34" s="14" t="s">
+        <v>97</v>
+      </c>
+      <c r="E34" s="14" t="s">
+        <v>98</v>
+      </c>
     </row>
     <row r="35" spans="2:5">
-      <c r="B35" s="2"/>
-      <c r="C35" s="2"/>
-      <c r="D35" s="15" t="s">
-        <v>48</v>
-      </c>
-      <c r="E35" s="15" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="36" spans="2:5">
-      <c r="B36" s="2"/>
-      <c r="C36" s="2"/>
-      <c r="D36" s="14" t="s">
-        <v>80</v>
-      </c>
-      <c r="E36" s="14" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="37" spans="2:5" ht="45">
+      <c r="B35" s="2">
+        <v>2</v>
+      </c>
+      <c r="C35" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D35" s="2"/>
+      <c r="E35" s="2"/>
+    </row>
+    <row r="36" spans="2:5" ht="18.75">
+      <c r="B36" s="2">
+        <v>3</v>
+      </c>
+      <c r="C36" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D36" s="18" t="s">
+        <v>59</v>
+      </c>
+      <c r="E36" s="2"/>
+    </row>
+    <row r="37" spans="2:5">
       <c r="B37" s="2"/>
       <c r="C37" s="2"/>
-      <c r="D37" s="74" t="s">
-        <v>420</v>
-      </c>
-      <c r="E37" s="14" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="38" spans="2:5" ht="30">
+      <c r="D37" s="101" t="s">
+        <v>60</v>
+      </c>
+      <c r="E37" s="101"/>
+    </row>
+    <row r="38" spans="2:5">
       <c r="B38" s="2"/>
       <c r="C38" s="2"/>
-      <c r="D38" s="74" t="s">
-        <v>421</v>
-      </c>
-      <c r="E38" s="14" t="s">
-        <v>84</v>
+      <c r="D38" s="15" t="s">
+        <v>61</v>
+      </c>
+      <c r="E38" s="15" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="39" spans="2:5" ht="30">
       <c r="B39" s="2"/>
       <c r="C39" s="2"/>
-      <c r="D39" s="74" t="s">
-        <v>422</v>
+      <c r="D39" s="14" t="s">
+        <v>63</v>
       </c>
       <c r="E39" s="14" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="40" spans="2:5" ht="18.75">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="40" spans="2:5">
       <c r="B40" s="2"/>
       <c r="C40" s="2"/>
-      <c r="D40" s="20" t="s">
-        <v>85</v>
-      </c>
-      <c r="E40" s="20"/>
+      <c r="D40" s="14" t="s">
+        <v>65</v>
+      </c>
+      <c r="E40" s="14" t="s">
+        <v>66</v>
+      </c>
     </row>
     <row r="41" spans="2:5">
       <c r="B41" s="2"/>
       <c r="C41" s="2"/>
-      <c r="D41" s="96" t="s">
-        <v>86</v>
-      </c>
-      <c r="E41" s="97"/>
+      <c r="D41" s="14" t="s">
+        <v>67</v>
+      </c>
+      <c r="E41" s="14" t="s">
+        <v>68</v>
+      </c>
     </row>
     <row r="42" spans="2:5">
       <c r="B42" s="2"/>
       <c r="C42" s="2"/>
-      <c r="D42" s="15" t="s">
-        <v>87</v>
-      </c>
-      <c r="E42" s="15" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="43" spans="2:5" ht="45">
+      <c r="D42" s="14" t="s">
+        <v>69</v>
+      </c>
+      <c r="E42" s="102" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="43" spans="2:5">
       <c r="B43" s="2"/>
       <c r="C43" s="2"/>
       <c r="D43" s="14" t="s">
-        <v>89</v>
-      </c>
-      <c r="E43" s="14" t="s">
-        <v>90</v>
-      </c>
+        <v>70</v>
+      </c>
+      <c r="E43" s="102"/>
     </row>
     <row r="44" spans="2:5">
       <c r="B44" s="2"/>
       <c r="C44" s="2"/>
       <c r="D44" s="14" t="s">
-        <v>91</v>
+        <v>72</v>
       </c>
       <c r="E44" s="14" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="45" spans="2:5">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="45" spans="2:5" ht="60">
       <c r="B45" s="2"/>
       <c r="C45" s="2"/>
-      <c r="D45" s="14" t="s">
-        <v>93</v>
+      <c r="D45" s="74" t="s">
+        <v>423</v>
       </c>
       <c r="E45" s="14" t="s">
-        <v>94</v>
+        <v>74</v>
       </c>
     </row>
     <row r="46" spans="2:5">
       <c r="B46" s="2"/>
       <c r="C46" s="2"/>
       <c r="D46" s="14" t="s">
-        <v>95</v>
+        <v>75</v>
       </c>
       <c r="E46" s="14" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="47" spans="2:5" ht="30">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="47" spans="2:5">
       <c r="B47" s="2"/>
       <c r="C47" s="2"/>
-      <c r="D47" s="14" t="s">
-        <v>97</v>
-      </c>
-      <c r="E47" s="14" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="48" spans="2:5">
-      <c r="B48" s="2">
-        <v>2</v>
-      </c>
-      <c r="C48" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="D48" s="2"/>
-      <c r="E48" s="2"/>
-    </row>
-    <row r="49" spans="2:5" ht="18.75">
-      <c r="B49" s="2">
-        <v>3</v>
-      </c>
-      <c r="C49" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="D49" s="18" t="s">
-        <v>59</v>
-      </c>
-      <c r="E49" s="2"/>
-    </row>
-    <row r="50" spans="2:5">
+      <c r="D47" s="73"/>
+      <c r="E47" s="73"/>
+    </row>
+    <row r="48" spans="2:5" ht="31.5">
+      <c r="B48" s="2"/>
+      <c r="C48" s="2"/>
+      <c r="D48" s="22" t="s">
+        <v>414</v>
+      </c>
+      <c r="E48" s="73"/>
+    </row>
+    <row r="49" spans="2:5" ht="18" customHeight="1">
+      <c r="B49" s="2"/>
+      <c r="C49" s="2"/>
+      <c r="D49" s="69" t="s">
+        <v>416</v>
+      </c>
+      <c r="E49" s="69" t="s">
+        <v>415</v>
+      </c>
+    </row>
+    <row r="50" spans="2:5" ht="62.25" customHeight="1">
       <c r="B50" s="2"/>
       <c r="C50" s="2"/>
-      <c r="D50" s="93" t="s">
-        <v>60</v>
-      </c>
-      <c r="E50" s="93"/>
+      <c r="D50" s="13" t="s">
+        <v>419</v>
+      </c>
+      <c r="E50" s="77" t="s">
+        <v>417</v>
+      </c>
     </row>
     <row r="51" spans="2:5">
       <c r="B51" s="2"/>
       <c r="C51" s="2"/>
-      <c r="D51" s="15" t="s">
-        <v>61</v>
-      </c>
-      <c r="E51" s="15" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="52" spans="2:5" ht="30">
+      <c r="D51" s="13"/>
+      <c r="E51" s="13"/>
+    </row>
+    <row r="52" spans="2:5" ht="31.5">
       <c r="B52" s="2"/>
       <c r="C52" s="2"/>
-      <c r="D52" s="14" t="s">
-        <v>63</v>
-      </c>
-      <c r="E52" s="14" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="53" spans="2:5">
+      <c r="D52" s="22" t="s">
+        <v>418</v>
+      </c>
+      <c r="E52" s="73"/>
+    </row>
+    <row r="53" spans="2:5" ht="150">
       <c r="B53" s="2"/>
       <c r="C53" s="2"/>
-      <c r="D53" s="14" t="s">
-        <v>65</v>
-      </c>
-      <c r="E53" s="14" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="54" spans="2:5">
-      <c r="B54" s="2"/>
-      <c r="C54" s="2"/>
-      <c r="D54" s="14" t="s">
-        <v>67</v>
-      </c>
-      <c r="E54" s="14" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="55" spans="2:5">
-      <c r="B55" s="2"/>
-      <c r="C55" s="2"/>
-      <c r="D55" s="14" t="s">
-        <v>69</v>
-      </c>
-      <c r="E55" s="94" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="56" spans="2:5">
+      <c r="D53" s="73" t="s">
+        <v>413</v>
+      </c>
+      <c r="E53" s="2"/>
+    </row>
+    <row r="55" spans="2:5" ht="31.5">
+      <c r="B55" s="22" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="56" spans="2:5" ht="49.5" customHeight="1">
       <c r="B56" s="2"/>
       <c r="C56" s="2"/>
-      <c r="D56" s="14" t="s">
-        <v>70</v>
-      </c>
-      <c r="E56" s="94"/>
-    </row>
-    <row r="57" spans="2:5">
+      <c r="D56" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="E56" s="25" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="57" spans="2:5" ht="45">
       <c r="B57" s="2"/>
       <c r="C57" s="2"/>
-      <c r="D57" s="14" t="s">
-        <v>72</v>
-      </c>
-      <c r="E57" s="14" t="s">
-        <v>73</v>
+      <c r="D57" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="E57" s="17" t="s">
+        <v>111</v>
       </c>
     </row>
     <row r="58" spans="2:5" ht="60">
       <c r="B58" s="2"/>
       <c r="C58" s="2"/>
-      <c r="D58" s="74" t="s">
-        <v>423</v>
-      </c>
-      <c r="E58" s="14" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="59" spans="2:5">
+      <c r="D58" t="s">
+        <v>106</v>
+      </c>
+      <c r="E58" s="13" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="59" spans="2:5" ht="45">
       <c r="B59" s="2"/>
       <c r="C59" s="2"/>
-      <c r="D59" s="14" t="s">
-        <v>75</v>
-      </c>
-      <c r="E59" s="14" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="60" spans="2:5">
+      <c r="D59" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="E59" s="17" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="60" spans="2:5" ht="45">
       <c r="B60" s="2"/>
       <c r="C60" s="2"/>
-      <c r="D60" s="73"/>
-      <c r="E60" s="73"/>
-    </row>
-    <row r="61" spans="2:5" ht="31.5">
+      <c r="D60" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="E60" s="17" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="61" spans="2:5" ht="30">
       <c r="B61" s="2"/>
       <c r="C61" s="2"/>
-      <c r="D61" s="22" t="s">
-        <v>414</v>
-      </c>
-      <c r="E61" s="73"/>
-    </row>
-    <row r="62" spans="2:5" ht="18" customHeight="1">
+      <c r="D61" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="E61" s="17" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="62" spans="2:5" ht="30">
       <c r="B62" s="2"/>
       <c r="C62" s="2"/>
-      <c r="D62" s="69" t="s">
-        <v>416</v>
-      </c>
-      <c r="E62" s="69" t="s">
-        <v>415</v>
-      </c>
-    </row>
-    <row r="63" spans="2:5" ht="62.25" customHeight="1">
+      <c r="D62" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="E62" s="72" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="63" spans="2:5" ht="120">
       <c r="B63" s="2"/>
       <c r="C63" s="2"/>
-      <c r="D63" s="13" t="s">
-        <v>419</v>
-      </c>
-      <c r="E63" s="77" t="s">
-        <v>417</v>
-      </c>
-    </row>
-    <row r="64" spans="2:5">
+      <c r="D63" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="E63" s="17" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="64" spans="2:5" ht="60">
       <c r="B64" s="2"/>
       <c r="C64" s="2"/>
-      <c r="D64" s="13"/>
-      <c r="E64" s="13"/>
-    </row>
-    <row r="65" spans="2:5" ht="31.5">
-      <c r="B65" s="2"/>
-      <c r="C65" s="2"/>
-      <c r="D65" s="22" t="s">
-        <v>418</v>
-      </c>
-      <c r="E65" s="73"/>
-    </row>
-    <row r="66" spans="2:5" ht="150">
-      <c r="B66" s="2"/>
-      <c r="C66" s="2"/>
-      <c r="D66" s="73" t="s">
-        <v>413</v>
-      </c>
-      <c r="E66" s="2"/>
-    </row>
-    <row r="68" spans="2:5" ht="31.5">
-      <c r="B68" s="22" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="69" spans="2:5" ht="49.5" customHeight="1">
-      <c r="B69" s="2"/>
+      <c r="D64" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="E64" s="17" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="66" spans="2:5" ht="31.5">
+      <c r="B66" s="22" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="67" spans="2:5" ht="53.25" customHeight="1">
+      <c r="B67" s="32"/>
+      <c r="C67" s="2"/>
+      <c r="D67" s="2" t="s">
+        <v>436</v>
+      </c>
+      <c r="E67" s="74" t="s">
+        <v>437</v>
+      </c>
+    </row>
+    <row r="68" spans="2:5" ht="53.25" customHeight="1">
+      <c r="B68" s="32"/>
+      <c r="C68" s="2"/>
+      <c r="D68" s="2" t="s">
+        <v>438</v>
+      </c>
+      <c r="E68" s="74" t="s">
+        <v>439</v>
+      </c>
+    </row>
+    <row r="69" spans="2:5" ht="53.25" customHeight="1">
+      <c r="B69" s="32"/>
       <c r="C69" s="2"/>
       <c r="D69" s="2" t="s">
-        <v>103</v>
-      </c>
-      <c r="E69" s="25" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="70" spans="2:5" ht="45">
-      <c r="B70" s="2"/>
+        <v>440</v>
+      </c>
+      <c r="E69" s="74" t="s">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="70" spans="2:5" ht="205.5" customHeight="1">
+      <c r="B70" s="32"/>
       <c r="C70" s="2"/>
-      <c r="D70" s="2" t="s">
-        <v>105</v>
-      </c>
-      <c r="E70" s="17" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="71" spans="2:5" ht="60">
-      <c r="B71" s="2"/>
-      <c r="C71" s="2"/>
-      <c r="D71" t="s">
-        <v>106</v>
-      </c>
-      <c r="E71" s="13" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="72" spans="2:5" ht="45">
-      <c r="B72" s="2"/>
+      <c r="D70" s="78" t="s">
+        <v>442</v>
+      </c>
+      <c r="E70" s="13" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="71" spans="2:5" ht="35.25" customHeight="1">
+      <c r="B71" s="32"/>
+      <c r="C71" s="22" t="s">
+        <v>445</v>
+      </c>
+      <c r="D71" s="78"/>
+      <c r="E71" s="13"/>
+    </row>
+    <row r="72" spans="2:5" ht="52.5" customHeight="1">
+      <c r="B72" s="32"/>
       <c r="C72" s="2"/>
-      <c r="D72" s="2" t="s">
-        <v>108</v>
-      </c>
-      <c r="E72" s="17" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="73" spans="2:5" ht="45">
-      <c r="B73" s="2"/>
+      <c r="D72" s="78" t="s">
+        <v>446</v>
+      </c>
+      <c r="E72" s="13" t="s">
+        <v>444</v>
+      </c>
+    </row>
+    <row r="73" spans="2:5" ht="52.5" customHeight="1">
+      <c r="B73" s="32"/>
       <c r="C73" s="2"/>
-      <c r="D73" s="2" t="s">
-        <v>107</v>
-      </c>
-      <c r="E73" s="17" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="74" spans="2:5" ht="30">
-      <c r="B74" s="2"/>
+      <c r="D73" s="78" t="s">
+        <v>447</v>
+      </c>
+      <c r="E73" s="13" t="s">
+        <v>453</v>
+      </c>
+    </row>
+    <row r="74" spans="2:5" ht="36" customHeight="1">
+      <c r="B74" s="32"/>
       <c r="C74" s="2"/>
-      <c r="D74" s="2" t="s">
-        <v>109</v>
-      </c>
-      <c r="E74" s="17" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="75" spans="2:5" ht="30">
-      <c r="B75" s="2"/>
+      <c r="D74" s="78" t="s">
+        <v>449</v>
+      </c>
+      <c r="E74" s="13" t="s">
+        <v>448</v>
+      </c>
+    </row>
+    <row r="75" spans="2:5" ht="120.75" customHeight="1">
+      <c r="B75" s="32"/>
       <c r="C75" s="2"/>
-      <c r="D75" s="2" t="s">
-        <v>115</v>
-      </c>
-      <c r="E75" s="72" t="s">
-        <v>397</v>
-      </c>
-    </row>
-    <row r="76" spans="2:5" ht="120">
-      <c r="B76" s="2"/>
+      <c r="D75" s="78" t="s">
+        <v>450</v>
+      </c>
+      <c r="E75" s="13" t="s">
+        <v>454</v>
+      </c>
+    </row>
+    <row r="76" spans="2:5" ht="31.5">
+      <c r="B76" s="32"/>
       <c r="C76" s="2"/>
-      <c r="D76" s="2" t="s">
-        <v>116</v>
-      </c>
-      <c r="E76" s="17" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="77" spans="2:5" ht="60">
-      <c r="B77" s="2"/>
+      <c r="D76" s="80" t="s">
+        <v>451</v>
+      </c>
+      <c r="E76" s="13"/>
+    </row>
+    <row r="77" spans="2:5" ht="66" customHeight="1">
+      <c r="B77" s="32"/>
       <c r="C77" s="2"/>
-      <c r="D77" s="2" t="s">
-        <v>118</v>
-      </c>
-      <c r="E77" s="17" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="79" spans="2:5" ht="31.5">
-      <c r="B79" s="22" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="80" spans="2:5" ht="53.25" customHeight="1">
-      <c r="B80" s="32"/>
+      <c r="D77" s="79" t="s">
+        <v>452</v>
+      </c>
+      <c r="E77" s="13"/>
+    </row>
+    <row r="78" spans="2:5" ht="225">
+      <c r="B78" s="2"/>
+      <c r="C78" s="2"/>
+      <c r="D78" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="E78" s="21" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="79" spans="2:5">
+      <c r="B79" s="2"/>
+      <c r="C79" s="2"/>
+      <c r="D79" s="2"/>
+      <c r="E79" s="74"/>
+    </row>
+    <row r="80" spans="2:5" ht="30">
+      <c r="B80" s="2"/>
       <c r="C80" s="2"/>
       <c r="D80" s="2" t="s">
-        <v>436</v>
-      </c>
-      <c r="E80" s="74" t="s">
-        <v>437</v>
-      </c>
-    </row>
-    <row r="81" spans="2:5" ht="53.25" customHeight="1">
-      <c r="B81" s="32"/>
+        <v>122</v>
+      </c>
+      <c r="E80" s="17" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="81" spans="2:5" ht="90">
+      <c r="B81" s="2"/>
       <c r="C81" s="2"/>
       <c r="D81" s="2" t="s">
-        <v>438</v>
-      </c>
-      <c r="E81" s="74" t="s">
-        <v>439</v>
-      </c>
-    </row>
-    <row r="82" spans="2:5" ht="53.25" customHeight="1">
-      <c r="B82" s="32"/>
+        <v>121</v>
+      </c>
+      <c r="E81" s="17" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="82" spans="2:5" ht="45">
+      <c r="B82" s="2"/>
       <c r="C82" s="2"/>
       <c r="D82" s="2" t="s">
-        <v>440</v>
-      </c>
-      <c r="E82" s="74" t="s">
-        <v>441</v>
-      </c>
-    </row>
-    <row r="83" spans="2:5" ht="205.5" customHeight="1">
-      <c r="B83" s="32"/>
+        <v>126</v>
+      </c>
+      <c r="E82" s="21" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="83" spans="2:5" ht="60">
+      <c r="B83" s="2"/>
       <c r="C83" s="2"/>
-      <c r="D83" s="78" t="s">
-        <v>442</v>
-      </c>
-      <c r="E83" s="13" t="s">
-        <v>443</v>
-      </c>
-    </row>
-    <row r="84" spans="2:5" ht="35.25" customHeight="1">
-      <c r="B84" s="32"/>
-      <c r="C84" s="22" t="s">
-        <v>445</v>
-      </c>
-      <c r="D84" s="78"/>
-      <c r="E84" s="13"/>
-    </row>
-    <row r="85" spans="2:5" ht="52.5" customHeight="1">
-      <c r="B85" s="32"/>
+      <c r="D83" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="E83" s="21" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="84" spans="2:5" ht="90">
+      <c r="B84" s="2"/>
+      <c r="C84" s="2"/>
+      <c r="D84" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="E84" s="21" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="85" spans="2:5" ht="30">
+      <c r="B85" s="2"/>
       <c r="C85" s="2"/>
-      <c r="D85" s="78" t="s">
-        <v>446</v>
-      </c>
-      <c r="E85" s="13" t="s">
-        <v>444</v>
-      </c>
-    </row>
-    <row r="86" spans="2:5" ht="52.5" customHeight="1">
-      <c r="B86" s="32"/>
+      <c r="D85" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="E85" s="21" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="86" spans="2:5" ht="30">
+      <c r="B86" s="2"/>
       <c r="C86" s="2"/>
-      <c r="D86" s="78" t="s">
-        <v>447</v>
-      </c>
-      <c r="E86" s="13" t="s">
-        <v>453</v>
-      </c>
-    </row>
-    <row r="87" spans="2:5" ht="36" customHeight="1">
-      <c r="B87" s="32"/>
+      <c r="D86" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="E86" s="21" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="87" spans="2:5" ht="60">
+      <c r="B87" s="2"/>
       <c r="C87" s="2"/>
-      <c r="D87" s="78" t="s">
-        <v>449</v>
-      </c>
-      <c r="E87" s="13" t="s">
-        <v>448</v>
-      </c>
-    </row>
-    <row r="88" spans="2:5" ht="120.75" customHeight="1">
-      <c r="B88" s="32"/>
+      <c r="D87" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="E87" s="21" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="88" spans="2:5" ht="90">
+      <c r="B88" s="2"/>
       <c r="C88" s="2"/>
-      <c r="D88" s="78" t="s">
-        <v>450</v>
-      </c>
-      <c r="E88" s="13" t="s">
-        <v>454</v>
-      </c>
-    </row>
-    <row r="89" spans="2:5" ht="31.5">
-      <c r="B89" s="32"/>
+      <c r="D88" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="E88" s="21" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="89" spans="2:5" ht="60">
+      <c r="B89" s="2"/>
       <c r="C89" s="2"/>
-      <c r="D89" s="80" t="s">
-        <v>451</v>
-      </c>
-      <c r="E89" s="13"/>
-    </row>
-    <row r="90" spans="2:5" ht="66" customHeight="1">
-      <c r="B90" s="32"/>
+      <c r="D89" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="E89" s="21" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="90" spans="2:5">
+      <c r="B90" s="2"/>
       <c r="C90" s="2"/>
-      <c r="D90" s="79" t="s">
-        <v>452</v>
-      </c>
-      <c r="E90" s="13"/>
-    </row>
-    <row r="91" spans="2:5" ht="225">
+      <c r="D90" s="2"/>
+      <c r="E90" s="21"/>
+    </row>
+    <row r="91" spans="2:5">
       <c r="B91" s="2"/>
       <c r="C91" s="2"/>
-      <c r="D91" s="2" t="s">
-        <v>120</v>
-      </c>
-      <c r="E91" s="21" t="s">
-        <v>141</v>
-      </c>
+      <c r="D91" s="2"/>
+      <c r="E91" s="21"/>
     </row>
     <row r="92" spans="2:5">
       <c r="B92" s="2"/>
       <c r="C92" s="2"/>
       <c r="D92" s="2"/>
-      <c r="E92" s="74"/>
-    </row>
-    <row r="93" spans="2:5" ht="30">
+      <c r="E92" s="21"/>
+    </row>
+    <row r="93" spans="2:5">
       <c r="B93" s="2"/>
       <c r="C93" s="2"/>
-      <c r="D93" s="2" t="s">
-        <v>122</v>
-      </c>
-      <c r="E93" s="17" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="94" spans="2:5" ht="90">
+      <c r="D93" s="2"/>
+      <c r="E93" s="21"/>
+    </row>
+    <row r="94" spans="2:5">
       <c r="B94" s="2"/>
       <c r="C94" s="2"/>
-      <c r="D94" s="2" t="s">
-        <v>121</v>
-      </c>
-      <c r="E94" s="17" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="95" spans="2:5" ht="45">
+      <c r="D94" s="2"/>
+      <c r="E94" s="21"/>
+    </row>
+    <row r="95" spans="2:5">
       <c r="B95" s="2"/>
       <c r="C95" s="2"/>
-      <c r="D95" s="2" t="s">
-        <v>126</v>
-      </c>
-      <c r="E95" s="21" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="96" spans="2:5" ht="60">
+      <c r="D95" s="2"/>
+      <c r="E95" s="21"/>
+    </row>
+    <row r="96" spans="2:5">
       <c r="B96" s="2"/>
       <c r="C96" s="2"/>
-      <c r="D96" s="2" t="s">
-        <v>127</v>
-      </c>
-      <c r="E96" s="21" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="97" spans="2:5" ht="90">
+      <c r="D96" s="2"/>
+      <c r="E96" s="26"/>
+    </row>
+    <row r="97" spans="2:5">
       <c r="B97" s="2"/>
       <c r="C97" s="2"/>
-      <c r="D97" s="2" t="s">
-        <v>130</v>
-      </c>
-      <c r="E97" s="21" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="98" spans="2:5" ht="30">
+      <c r="D97" s="2"/>
+      <c r="E97" s="2"/>
+    </row>
+    <row r="98" spans="2:5">
       <c r="B98" s="2"/>
       <c r="C98" s="2"/>
-      <c r="D98" s="2" t="s">
-        <v>132</v>
-      </c>
-      <c r="E98" s="21" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="99" spans="2:5" ht="30">
+      <c r="D98" s="2"/>
+      <c r="E98" s="2"/>
+    </row>
+    <row r="99" spans="2:5">
       <c r="B99" s="2"/>
       <c r="C99" s="2"/>
-      <c r="D99" s="2" t="s">
-        <v>134</v>
-      </c>
-      <c r="E99" s="21" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="100" spans="2:5" ht="60">
+      <c r="D99" s="2"/>
+      <c r="E99" s="2"/>
+    </row>
+    <row r="100" spans="2:5">
       <c r="B100" s="2"/>
       <c r="C100" s="2"/>
-      <c r="D100" s="2" t="s">
-        <v>137</v>
-      </c>
-      <c r="E100" s="21" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="101" spans="2:5" ht="90">
+      <c r="D100" s="2"/>
+      <c r="E100" s="2"/>
+    </row>
+    <row r="101" spans="2:5" ht="60">
       <c r="B101" s="2"/>
       <c r="C101" s="2"/>
       <c r="D101" s="2" t="s">
-        <v>138</v>
-      </c>
-      <c r="E101" s="21" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="102" spans="2:5" ht="60">
+        <v>150</v>
+      </c>
+      <c r="E101" s="26" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="102" spans="2:5" ht="75">
       <c r="B102" s="2"/>
       <c r="C102" s="2"/>
       <c r="D102" s="2" t="s">
-        <v>140</v>
-      </c>
-      <c r="E102" s="21" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="103" spans="2:5">
+        <v>152</v>
+      </c>
+      <c r="E102" s="26" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="103" spans="2:5" ht="60">
       <c r="B103" s="2"/>
       <c r="C103" s="2"/>
-      <c r="D103" s="2"/>
-      <c r="E103" s="21"/>
-    </row>
-    <row r="104" spans="2:5">
+      <c r="D103" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="E103" s="26" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="104" spans="2:5" ht="32.25" customHeight="1">
       <c r="B104" s="2"/>
       <c r="C104" s="2"/>
-      <c r="D104" s="2"/>
-      <c r="E104" s="21"/>
+      <c r="D104" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="E104" s="26" t="s">
+        <v>159</v>
+      </c>
     </row>
     <row r="105" spans="2:5">
       <c r="B105" s="2"/>
       <c r="C105" s="2"/>
-      <c r="D105" s="2"/>
-      <c r="E105" s="21"/>
-    </row>
-    <row r="106" spans="2:5">
+      <c r="D105" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="E105" s="26" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="106" spans="2:5" ht="75">
       <c r="B106" s="2"/>
       <c r="C106" s="2"/>
-      <c r="D106" s="2"/>
-      <c r="E106" s="21"/>
-    </row>
-    <row r="107" spans="2:5">
+      <c r="D106" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="E106" s="26" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="107" spans="2:5" ht="45">
       <c r="B107" s="2"/>
-      <c r="C107" s="2"/>
+      <c r="C107" s="32" t="s">
+        <v>425</v>
+      </c>
       <c r="D107" s="2"/>
-      <c r="E107" s="21"/>
-    </row>
-    <row r="108" spans="2:5">
+      <c r="E107" s="40" t="s">
+        <v>426</v>
+      </c>
+    </row>
+    <row r="108" spans="2:5" ht="31.5">
       <c r="B108" s="2"/>
-      <c r="C108" s="2"/>
+      <c r="C108" s="22"/>
       <c r="D108" s="2"/>
-      <c r="E108" s="21"/>
-    </row>
-    <row r="109" spans="2:5">
+      <c r="E108" s="74"/>
+    </row>
+    <row r="109" spans="2:5" ht="135">
       <c r="B109" s="2"/>
       <c r="C109" s="2"/>
-      <c r="D109" s="2"/>
-      <c r="E109" s="26"/>
-    </row>
-    <row r="110" spans="2:5">
+      <c r="D109" s="2" t="s">
+        <v>164</v>
+      </c>
+      <c r="E109" s="26" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="110" spans="2:5" ht="90">
       <c r="B110" s="2"/>
       <c r="C110" s="2"/>
-      <c r="D110" s="2"/>
-      <c r="E110" s="2"/>
-    </row>
-    <row r="111" spans="2:5">
+      <c r="D110" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="E110" s="26" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="111" spans="2:5" ht="45">
       <c r="B111" s="2"/>
       <c r="C111" s="2"/>
-      <c r="D111" s="2"/>
-      <c r="E111" s="2"/>
+      <c r="D111" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="E111" s="26" t="s">
+        <v>169</v>
+      </c>
     </row>
     <row r="112" spans="2:5">
       <c r="B112" s="2"/>
       <c r="C112" s="2"/>
-      <c r="D112" s="2"/>
-      <c r="E112" s="2"/>
-    </row>
-    <row r="113" spans="2:5">
+      <c r="D112" s="2" t="s">
+        <v>170</v>
+      </c>
+      <c r="E112" s="26" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="113" spans="2:5" ht="30">
       <c r="B113" s="2"/>
       <c r="C113" s="2"/>
-      <c r="D113" s="2"/>
-      <c r="E113" s="2"/>
-    </row>
-    <row r="114" spans="2:5" ht="60">
+      <c r="D113" s="26" t="s">
+        <v>172</v>
+      </c>
+      <c r="E113" s="26" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="114" spans="2:5">
       <c r="B114" s="2"/>
       <c r="C114" s="2"/>
       <c r="D114" s="2" t="s">
-        <v>150</v>
-      </c>
-      <c r="E114" s="26" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="115" spans="2:5" ht="75">
+        <v>174</v>
+      </c>
+      <c r="E114" s="26"/>
+    </row>
+    <row r="115" spans="2:5">
       <c r="B115" s="2"/>
       <c r="C115" s="2"/>
-      <c r="D115" s="2" t="s">
-        <v>152</v>
-      </c>
-      <c r="E115" s="26" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="116" spans="2:5" ht="60">
+      <c r="D115" s="15" t="s">
+        <v>175</v>
+      </c>
+      <c r="E115" s="15" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="116" spans="2:5">
       <c r="B116" s="2"/>
       <c r="C116" s="2"/>
-      <c r="D116" s="2" t="s">
-        <v>156</v>
+      <c r="D116" s="26" t="s">
+        <v>177</v>
       </c>
       <c r="E116" s="26" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="117" spans="2:5" ht="32.25" customHeight="1">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="117" spans="2:5">
       <c r="B117" s="2"/>
       <c r="C117" s="2"/>
-      <c r="D117" s="2" t="s">
-        <v>158</v>
+      <c r="D117" s="26" t="s">
+        <v>179</v>
       </c>
       <c r="E117" s="26" t="s">
-        <v>159</v>
+        <v>180</v>
       </c>
     </row>
     <row r="118" spans="2:5">
       <c r="B118" s="2"/>
       <c r="C118" s="2"/>
-      <c r="D118" s="2" t="s">
-        <v>160</v>
+      <c r="D118" s="26" t="s">
+        <v>181</v>
       </c>
       <c r="E118" s="26" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="119" spans="2:5" ht="75">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="119" spans="2:5">
       <c r="B119" s="2"/>
       <c r="C119" s="2"/>
-      <c r="D119" s="2" t="s">
-        <v>162</v>
+      <c r="D119" s="26" t="s">
+        <v>183</v>
       </c>
       <c r="E119" s="26" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="120" spans="2:5" ht="45">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="120" spans="2:5" ht="31.5">
       <c r="B120" s="2"/>
-      <c r="C120" s="32" t="s">
-        <v>425</v>
+      <c r="C120" s="22" t="s">
+        <v>185</v>
       </c>
       <c r="D120" s="2"/>
-      <c r="E120" s="40" t="s">
-        <v>426</v>
-      </c>
-    </row>
-    <row r="121" spans="2:5" ht="31.5">
+      <c r="E120" s="26"/>
+    </row>
+    <row r="121" spans="2:5" ht="105">
       <c r="B121" s="2"/>
-      <c r="C121" s="22"/>
-      <c r="D121" s="2"/>
-      <c r="E121" s="74"/>
-    </row>
-    <row r="122" spans="2:5" ht="135">
+      <c r="C121" s="2"/>
+      <c r="D121" s="2" t="s">
+        <v>186</v>
+      </c>
+      <c r="E121" s="74" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="122" spans="2:5" ht="120">
       <c r="B122" s="2"/>
       <c r="C122" s="2"/>
       <c r="D122" s="2" t="s">
-        <v>164</v>
-      </c>
-      <c r="E122" s="26" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="123" spans="2:5" ht="90">
+        <v>187</v>
+      </c>
+      <c r="E122" s="74" t="s">
+        <v>424</v>
+      </c>
+    </row>
+    <row r="123" spans="2:5" ht="255">
       <c r="B123" s="2"/>
       <c r="C123" s="2"/>
       <c r="D123" s="2" t="s">
-        <v>166</v>
+        <v>188</v>
       </c>
       <c r="E123" s="26" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="124" spans="2:5" ht="45">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="124" spans="2:5" ht="180">
       <c r="B124" s="2"/>
       <c r="C124" s="2"/>
       <c r="D124" s="2" t="s">
-        <v>168</v>
-      </c>
-      <c r="E124" s="26" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="125" spans="2:5">
+        <v>190</v>
+      </c>
+      <c r="E124" s="28" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="125" spans="2:5" ht="30">
       <c r="B125" s="2"/>
       <c r="C125" s="2"/>
-      <c r="D125" s="2" t="s">
-        <v>170</v>
-      </c>
-      <c r="E125" s="26" t="s">
-        <v>171</v>
-      </c>
+      <c r="D125" s="28" t="s">
+        <v>195</v>
+      </c>
+      <c r="E125" s="28"/>
     </row>
     <row r="126" spans="2:5" ht="30">
       <c r="B126" s="2"/>
       <c r="C126" s="2"/>
-      <c r="D126" s="26" t="s">
-        <v>172</v>
-      </c>
-      <c r="E126" s="26" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="127" spans="2:5">
+      <c r="D126" s="28" t="s">
+        <v>196</v>
+      </c>
+      <c r="E126" s="28"/>
+    </row>
+    <row r="127" spans="2:5" ht="30">
       <c r="B127" s="2"/>
       <c r="C127" s="2"/>
-      <c r="D127" s="2" t="s">
-        <v>174</v>
-      </c>
-      <c r="E127" s="26"/>
-    </row>
-    <row r="128" spans="2:5">
+      <c r="D127" s="28" t="s">
+        <v>198</v>
+      </c>
+      <c r="E127" s="28"/>
+    </row>
+    <row r="128" spans="2:5" ht="45">
       <c r="B128" s="2"/>
       <c r="C128" s="2"/>
-      <c r="D128" s="15" t="s">
-        <v>175</v>
-      </c>
-      <c r="E128" s="15" t="s">
-        <v>176</v>
-      </c>
+      <c r="D128" s="28" t="s">
+        <v>192</v>
+      </c>
+      <c r="E128" s="28"/>
     </row>
     <row r="129" spans="2:5">
       <c r="B129" s="2"/>
       <c r="C129" s="2"/>
-      <c r="D129" s="26" t="s">
-        <v>177</v>
-      </c>
-      <c r="E129" s="26" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="130" spans="2:5">
+      <c r="D129" s="28" t="s">
+        <v>199</v>
+      </c>
+      <c r="E129" s="28"/>
+    </row>
+    <row r="130" spans="2:5" ht="60">
       <c r="B130" s="2"/>
       <c r="C130" s="2"/>
-      <c r="D130" s="26" t="s">
-        <v>179</v>
-      </c>
-      <c r="E130" s="26" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="131" spans="2:5">
+      <c r="D130" s="28" t="s">
+        <v>200</v>
+      </c>
+      <c r="E130" s="28"/>
+    </row>
+    <row r="131" spans="2:5" ht="30">
       <c r="B131" s="2"/>
       <c r="C131" s="2"/>
-      <c r="D131" s="26" t="s">
-        <v>181</v>
-      </c>
-      <c r="E131" s="26" t="s">
-        <v>182</v>
-      </c>
+      <c r="D131" s="28" t="s">
+        <v>201</v>
+      </c>
+      <c r="E131" s="28"/>
     </row>
     <row r="132" spans="2:5">
       <c r="B132" s="2"/>
       <c r="C132" s="2"/>
-      <c r="D132" s="26" t="s">
-        <v>183</v>
-      </c>
-      <c r="E132" s="26" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="133" spans="2:5" ht="31.5">
+      <c r="D132" s="28" t="s">
+        <v>202</v>
+      </c>
+      <c r="E132" s="28"/>
+    </row>
+    <row r="133" spans="2:5" ht="30">
       <c r="B133" s="2"/>
-      <c r="C133" s="22" t="s">
-        <v>185</v>
-      </c>
-      <c r="D133" s="2"/>
-      <c r="E133" s="26"/>
-    </row>
-    <row r="134" spans="2:5" ht="105">
+      <c r="C133" s="2"/>
+      <c r="D133" s="28" t="s">
+        <v>193</v>
+      </c>
+      <c r="E133" s="28"/>
+    </row>
+    <row r="134" spans="2:5" ht="30">
       <c r="B134" s="2"/>
       <c r="C134" s="2"/>
-      <c r="D134" s="2" t="s">
-        <v>186</v>
-      </c>
-      <c r="E134" s="74" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="135" spans="2:5" ht="120">
+      <c r="D134" s="28" t="s">
+        <v>194</v>
+      </c>
+      <c r="E134" s="28"/>
+    </row>
+    <row r="135" spans="2:5">
       <c r="B135" s="2"/>
       <c r="C135" s="2"/>
-      <c r="D135" s="2" t="s">
-        <v>187</v>
-      </c>
-      <c r="E135" s="74" t="s">
-        <v>424</v>
-      </c>
-    </row>
-    <row r="136" spans="2:5" ht="255">
-      <c r="B136" s="2"/>
-      <c r="C136" s="2"/>
-      <c r="D136" s="2" t="s">
-        <v>188</v>
-      </c>
-      <c r="E136" s="26" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="137" spans="2:5" ht="180">
-      <c r="B137" s="2"/>
-      <c r="C137" s="2"/>
-      <c r="D137" s="2" t="s">
-        <v>190</v>
-      </c>
-      <c r="E137" s="28" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="138" spans="2:5" ht="30">
+      <c r="D135" s="28"/>
+      <c r="E135" s="26"/>
+    </row>
+    <row r="137" spans="2:5" ht="31.5">
+      <c r="C137" s="22" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="138" spans="2:5" ht="90">
       <c r="B138" s="2"/>
       <c r="C138" s="2"/>
-      <c r="D138" s="28" t="s">
-        <v>195</v>
-      </c>
-      <c r="E138" s="28"/>
-    </row>
-    <row r="139" spans="2:5" ht="30">
+      <c r="D138" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="E138" s="21" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="139" spans="2:5" ht="90">
       <c r="B139" s="2"/>
       <c r="C139" s="2"/>
       <c r="D139" s="28" t="s">
-        <v>196</v>
-      </c>
-      <c r="E139" s="28"/>
-    </row>
-    <row r="140" spans="2:5" ht="30">
+        <v>146</v>
+      </c>
+      <c r="E139" s="21" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="140" spans="2:5" ht="105">
       <c r="B140" s="2"/>
       <c r="C140" s="2"/>
-      <c r="D140" s="28" t="s">
-        <v>198</v>
-      </c>
-      <c r="E140" s="28"/>
-    </row>
-    <row r="141" spans="2:5" ht="45">
+      <c r="D140" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="E140" s="21" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="141" spans="2:5" ht="90">
       <c r="B141" s="2"/>
       <c r="C141" s="2"/>
-      <c r="D141" s="28" t="s">
-        <v>192</v>
-      </c>
-      <c r="E141" s="28"/>
+      <c r="D141" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="E141" s="21" t="s">
+        <v>149</v>
+      </c>
     </row>
     <row r="142" spans="2:5">
       <c r="B142" s="2"/>
       <c r="C142" s="2"/>
-      <c r="D142" s="28" t="s">
-        <v>199</v>
-      </c>
-      <c r="E142" s="28"/>
-    </row>
-    <row r="143" spans="2:5" ht="60">
+      <c r="D142" s="2"/>
+      <c r="E142" s="21"/>
+    </row>
+    <row r="143" spans="2:5">
       <c r="B143" s="2"/>
       <c r="C143" s="2"/>
-      <c r="D143" s="28" t="s">
-        <v>200</v>
-      </c>
-      <c r="E143" s="28"/>
-    </row>
-    <row r="144" spans="2:5" ht="30">
+      <c r="D143" s="2"/>
+      <c r="E143" s="21"/>
+    </row>
+    <row r="144" spans="2:5">
       <c r="B144" s="2"/>
       <c r="C144" s="2"/>
-      <c r="D144" s="28" t="s">
-        <v>201</v>
-      </c>
-      <c r="E144" s="28"/>
+      <c r="D144" s="2"/>
+      <c r="E144" s="21"/>
     </row>
     <row r="145" spans="2:5">
       <c r="B145" s="2"/>
       <c r="C145" s="2"/>
-      <c r="D145" s="28" t="s">
-        <v>202</v>
-      </c>
-      <c r="E145" s="28"/>
-    </row>
-    <row r="146" spans="2:5" ht="30">
+      <c r="D145" s="2"/>
+      <c r="E145" s="21"/>
+    </row>
+    <row r="146" spans="2:5">
       <c r="B146" s="2"/>
       <c r="C146" s="2"/>
-      <c r="D146" s="28" t="s">
-        <v>193</v>
-      </c>
-      <c r="E146" s="28"/>
-    </row>
-    <row r="147" spans="2:5" ht="30">
+      <c r="D146" s="2"/>
+      <c r="E146" s="21"/>
+    </row>
+    <row r="147" spans="2:5">
       <c r="B147" s="2"/>
       <c r="C147" s="2"/>
-      <c r="D147" s="28" t="s">
-        <v>194</v>
-      </c>
-      <c r="E147" s="28"/>
+      <c r="D147" s="2"/>
+      <c r="E147" s="21"/>
     </row>
     <row r="148" spans="2:5">
       <c r="B148" s="2"/>
       <c r="C148" s="2"/>
-      <c r="D148" s="28"/>
-      <c r="E148" s="26"/>
-    </row>
-    <row r="150" spans="2:5" ht="31.5">
-      <c r="C150" s="22" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="151" spans="2:5" ht="90">
-      <c r="B151" s="2"/>
-      <c r="C151" s="2"/>
-      <c r="D151" s="2" t="s">
-        <v>144</v>
-      </c>
-      <c r="E151" s="21" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="152" spans="2:5" ht="90">
-      <c r="B152" s="2"/>
-      <c r="C152" s="2"/>
-      <c r="D152" s="28" t="s">
-        <v>146</v>
-      </c>
-      <c r="E152" s="21" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="153" spans="2:5" ht="105">
-      <c r="B153" s="2"/>
-      <c r="C153" s="2"/>
-      <c r="D153" s="2" t="s">
-        <v>155</v>
-      </c>
-      <c r="E153" s="21" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="154" spans="2:5" ht="90">
-      <c r="B154" s="2"/>
-      <c r="C154" s="2"/>
-      <c r="D154" s="2" t="s">
-        <v>154</v>
-      </c>
-      <c r="E154" s="21" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="155" spans="2:5">
-      <c r="B155" s="2"/>
-      <c r="C155" s="2"/>
-      <c r="D155" s="2"/>
-      <c r="E155" s="21"/>
-    </row>
-    <row r="156" spans="2:5">
-      <c r="B156" s="2"/>
-      <c r="C156" s="2"/>
-      <c r="D156" s="2"/>
-      <c r="E156" s="21"/>
-    </row>
-    <row r="157" spans="2:5">
-      <c r="B157" s="2"/>
-      <c r="C157" s="2"/>
-      <c r="D157" s="2"/>
-      <c r="E157" s="21"/>
-    </row>
-    <row r="158" spans="2:5">
-      <c r="B158" s="2"/>
-      <c r="C158" s="2"/>
-      <c r="D158" s="2"/>
-      <c r="E158" s="21"/>
-    </row>
-    <row r="159" spans="2:5">
-      <c r="B159" s="2"/>
-      <c r="C159" s="2"/>
-      <c r="D159" s="2"/>
-      <c r="E159" s="21"/>
-    </row>
-    <row r="160" spans="2:5">
-      <c r="B160" s="2"/>
-      <c r="C160" s="2"/>
-      <c r="D160" s="2"/>
-      <c r="E160" s="21"/>
-    </row>
-    <row r="161" spans="2:5">
-      <c r="B161" s="2"/>
-      <c r="C161" s="2"/>
-      <c r="D161" s="2"/>
-      <c r="E161" s="21"/>
-    </row>
-    <row r="162" spans="2:5">
-      <c r="B162" s="2"/>
-      <c r="C162" s="2"/>
-      <c r="D162" s="2"/>
-      <c r="E162" s="21"/>
-    </row>
-    <row r="163" spans="2:5">
-      <c r="E163" s="27"/>
+      <c r="D148" s="2"/>
+      <c r="E148" s="21"/>
+    </row>
+    <row r="149" spans="2:5">
+      <c r="B149" s="2"/>
+      <c r="C149" s="2"/>
+      <c r="D149" s="2"/>
+      <c r="E149" s="21"/>
+    </row>
+    <row r="150" spans="2:5">
+      <c r="E150" s="27"/>
+    </row>
+    <row r="185" spans="2:5" ht="31.5">
+      <c r="B185" s="22" t="s">
+        <v>203</v>
+      </c>
+      <c r="C185" s="23"/>
+      <c r="D185" s="23"/>
+      <c r="E185" s="24"/>
+    </row>
+    <row r="186" spans="2:5">
+      <c r="B186" s="19" t="s">
+        <v>3</v>
+      </c>
+      <c r="C186" s="19"/>
+      <c r="D186" s="19" t="s">
+        <v>35</v>
+      </c>
+      <c r="E186" s="19" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="187" spans="2:5" ht="165">
+      <c r="B187" s="2"/>
+      <c r="C187" s="2"/>
+      <c r="D187" s="10" t="s">
+        <v>204</v>
+      </c>
+      <c r="E187" s="29" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="188" spans="2:5">
+      <c r="B188" s="2"/>
+      <c r="C188" s="2"/>
+      <c r="D188" s="31" t="s">
+        <v>206</v>
+      </c>
+      <c r="E188" s="31" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="189" spans="2:5">
+      <c r="B189" s="2"/>
+      <c r="C189" s="2"/>
+      <c r="D189" s="2" t="s">
+        <v>208</v>
+      </c>
+      <c r="E189" s="29" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="190" spans="2:5" ht="30">
+      <c r="B190" s="2"/>
+      <c r="C190" s="2"/>
+      <c r="D190" s="2" t="s">
+        <v>210</v>
+      </c>
+      <c r="E190" s="29" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="191" spans="2:5">
+      <c r="B191" s="2"/>
+      <c r="C191" s="2"/>
+      <c r="D191" s="2" t="s">
+        <v>212</v>
+      </c>
+      <c r="E191" s="29" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="192" spans="2:5">
+      <c r="B192" s="2"/>
+      <c r="C192" s="2"/>
+      <c r="D192" s="2" t="s">
+        <v>214</v>
+      </c>
+      <c r="E192" s="29" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="193" spans="2:5">
+      <c r="B193" s="2"/>
+      <c r="C193" s="2"/>
+      <c r="D193" s="2" t="s">
+        <v>216</v>
+      </c>
+      <c r="E193" s="29" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="194" spans="2:5" ht="74.25" customHeight="1">
+      <c r="B194" s="2"/>
+      <c r="C194" s="32"/>
+      <c r="D194" s="33" t="s">
+        <v>218</v>
+      </c>
+      <c r="E194" s="30" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="195" spans="2:5" ht="78.75">
+      <c r="B195" s="2"/>
+      <c r="C195" s="32"/>
+      <c r="D195" s="33" t="s">
+        <v>212</v>
+      </c>
+      <c r="E195" s="30" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="196" spans="2:5" ht="93.75">
+      <c r="B196" s="2"/>
+      <c r="C196" s="32"/>
+      <c r="D196" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="E196" s="30" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="197" spans="2:5">
+      <c r="B197" s="2"/>
+      <c r="C197" s="2"/>
+      <c r="D197" s="2"/>
+      <c r="E197" s="29"/>
     </row>
   </sheetData>
   <mergeCells count="5">
-    <mergeCell ref="D27:E27"/>
-    <mergeCell ref="D50:E50"/>
-    <mergeCell ref="E55:E56"/>
-    <mergeCell ref="D34:E34"/>
-    <mergeCell ref="D41:E41"/>
+    <mergeCell ref="D14:E14"/>
+    <mergeCell ref="D37:E37"/>
+    <mergeCell ref="E42:E43"/>
+    <mergeCell ref="D21:E21"/>
+    <mergeCell ref="D28:E28"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -13479,27 +13663,27 @@
       </c>
     </row>
     <row r="49" spans="1:3">
-      <c r="A49" s="94" t="s">
+      <c r="A49" s="102" t="s">
         <v>338</v>
       </c>
       <c r="B49" s="53" t="s">
         <v>339</v>
       </c>
-      <c r="C49" s="94" t="s">
+      <c r="C49" s="102" t="s">
         <v>341</v>
       </c>
     </row>
     <row r="50" spans="1:3">
-      <c r="A50" s="94"/>
+      <c r="A50" s="102"/>
       <c r="B50" s="53"/>
-      <c r="C50" s="94"/>
+      <c r="C50" s="102"/>
     </row>
     <row r="51" spans="1:3">
-      <c r="A51" s="94"/>
+      <c r="A51" s="102"/>
       <c r="B51" s="53" t="s">
         <v>340</v>
       </c>
-      <c r="C51" s="94"/>
+      <c r="C51" s="102"/>
     </row>
     <row r="52" spans="1:3">
       <c r="A52" s="53" t="s">
@@ -13529,22 +13713,22 @@
       <c r="B56" s="58"/>
     </row>
     <row r="57" spans="1:3" ht="32.25" customHeight="1">
-      <c r="B57" s="98" t="s">
+      <c r="B57" s="106" t="s">
         <v>347</v>
       </c>
-      <c r="C57" s="98"/>
+      <c r="C57" s="106"/>
     </row>
     <row r="58" spans="1:3" ht="33" customHeight="1">
-      <c r="B58" s="98" t="s">
+      <c r="B58" s="106" t="s">
         <v>348</v>
       </c>
-      <c r="C58" s="98"/>
+      <c r="C58" s="106"/>
     </row>
     <row r="59" spans="1:3" ht="19.5" customHeight="1">
-      <c r="B59" s="98" t="s">
+      <c r="B59" s="106" t="s">
         <v>349</v>
       </c>
-      <c r="C59" s="98"/>
+      <c r="C59" s="106"/>
     </row>
     <row r="60" spans="1:3">
       <c r="B60" s="2" t="s">
@@ -13757,10 +13941,10 @@
       <c r="C87" s="76"/>
     </row>
     <row r="88" spans="1:3" ht="51" customHeight="1">
-      <c r="B88" s="98" t="s">
+      <c r="B88" s="106" t="s">
         <v>400</v>
       </c>
-      <c r="C88" s="98"/>
+      <c r="C88" s="106"/>
     </row>
     <row r="89" spans="1:3" ht="31.5">
       <c r="B89" s="22" t="s">
@@ -13771,13 +13955,13 @@
       <c r="A90" t="s">
         <v>402</v>
       </c>
-      <c r="B90" s="98" t="s">
+      <c r="B90" s="106" t="s">
         <v>401</v>
       </c>
-      <c r="C90" s="98"/>
+      <c r="C90" s="106"/>
     </row>
     <row r="91" spans="1:3" ht="45.75" customHeight="1">
-      <c r="A91" s="99" t="s">
+      <c r="A91" s="107" t="s">
         <v>405</v>
       </c>
       <c r="B91" s="2" t="s">
@@ -13788,7 +13972,7 @@
       </c>
     </row>
     <row r="92" spans="1:3" ht="30">
-      <c r="A92" s="99"/>
+      <c r="A92" s="107"/>
       <c r="B92" s="2" t="s">
         <v>408</v>
       </c>
@@ -13889,7 +14073,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B2:C128"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A100" workbookViewId="0">
+    <sheetView topLeftCell="A100" workbookViewId="0">
       <selection activeCell="B132" sqref="B132"/>
     </sheetView>
   </sheetViews>
@@ -14097,16 +14281,16 @@
       <c r="C26" s="37"/>
     </row>
     <row r="27" spans="2:3" ht="33" customHeight="1">
-      <c r="B27" s="100" t="s">
+      <c r="B27" s="108" t="s">
         <v>294</v>
       </c>
-      <c r="C27" s="100"/>
+      <c r="C27" s="108"/>
     </row>
     <row r="28" spans="2:3">
-      <c r="B28" s="100" t="s">
+      <c r="B28" s="108" t="s">
         <v>295</v>
       </c>
-      <c r="C28" s="100"/>
+      <c r="C28" s="108"/>
     </row>
     <row r="29" spans="2:3" ht="15.75" thickBot="1">
       <c r="B29" s="48" t="s">
@@ -14161,16 +14345,16 @@
       <c r="C37" s="51"/>
     </row>
     <row r="38" spans="2:3" ht="50.25" customHeight="1">
-      <c r="B38" s="100" t="s">
+      <c r="B38" s="108" t="s">
         <v>303</v>
       </c>
-      <c r="C38" s="100"/>
+      <c r="C38" s="108"/>
     </row>
     <row r="39" spans="2:3" ht="32.25" customHeight="1">
-      <c r="B39" s="100" t="s">
+      <c r="B39" s="108" t="s">
         <v>304</v>
       </c>
-      <c r="C39" s="100"/>
+      <c r="C39" s="108"/>
     </row>
     <row r="40" spans="2:3" ht="15.75" thickBot="1">
       <c r="B40" s="52" t="s">
@@ -14220,227 +14404,227 @@
       </c>
     </row>
     <row r="49" spans="2:3" ht="36" customHeight="1">
-      <c r="B49" s="100" t="s">
+      <c r="B49" s="108" t="s">
         <v>314</v>
       </c>
-      <c r="C49" s="100"/>
+      <c r="C49" s="108"/>
     </row>
     <row r="50" spans="2:3" ht="49.5" customHeight="1">
-      <c r="B50" s="100" t="s">
+      <c r="B50" s="108" t="s">
         <v>315</v>
       </c>
-      <c r="C50" s="100"/>
+      <c r="C50" s="108"/>
     </row>
     <row r="52" spans="2:3" ht="41.25">
-      <c r="B52" s="101" t="s">
+      <c r="B52" s="91" t="s">
         <v>479</v>
       </c>
     </row>
     <row r="53" spans="2:3">
-      <c r="B53" s="102" t="s">
+      <c r="B53" s="92" t="s">
         <v>480</v>
       </c>
     </row>
     <row r="54" spans="2:3">
-      <c r="B54" s="103" t="s">
+      <c r="B54" s="93" t="s">
         <v>481</v>
       </c>
     </row>
     <row r="55" spans="2:3">
-      <c r="B55" s="103" t="s">
+      <c r="B55" s="93" t="s">
         <v>482</v>
       </c>
     </row>
     <row r="56" spans="2:3">
-      <c r="B56" s="103" t="s">
+      <c r="B56" s="93" t="s">
         <v>483</v>
       </c>
     </row>
     <row r="57" spans="2:3">
-      <c r="B57" s="104" t="s">
+      <c r="B57" s="94" t="s">
         <v>484</v>
       </c>
     </row>
     <row r="58" spans="2:3">
-      <c r="B58" s="105"/>
+      <c r="B58" s="95"/>
     </row>
     <row r="59" spans="2:3">
-      <c r="B59" s="106" t="s">
+      <c r="B59" s="96" t="s">
         <v>485</v>
       </c>
     </row>
     <row r="60" spans="2:3">
-      <c r="B60" s="106" t="s">
+      <c r="B60" s="96" t="s">
         <v>486</v>
       </c>
     </row>
     <row r="61" spans="2:3">
-      <c r="B61" s="106" t="s">
+      <c r="B61" s="96" t="s">
         <v>487</v>
       </c>
     </row>
     <row r="62" spans="2:3">
-      <c r="B62" s="106" t="s">
+      <c r="B62" s="96" t="s">
         <v>488</v>
       </c>
     </row>
     <row r="63" spans="2:3">
-      <c r="B63" s="105"/>
+      <c r="B63" s="95"/>
     </row>
     <row r="64" spans="2:3">
-      <c r="B64" s="106" t="s">
+      <c r="B64" s="96" t="s">
         <v>485</v>
       </c>
     </row>
     <row r="65" spans="2:2">
-      <c r="B65" s="106" t="s">
+      <c r="B65" s="96" t="s">
         <v>489</v>
       </c>
     </row>
     <row r="66" spans="2:2">
-      <c r="B66" s="106" t="s">
+      <c r="B66" s="96" t="s">
         <v>490</v>
       </c>
     </row>
     <row r="67" spans="2:2">
-      <c r="B67" s="106" t="s">
+      <c r="B67" s="96" t="s">
         <v>488</v>
       </c>
     </row>
     <row r="68" spans="2:2">
-      <c r="B68" s="105"/>
+      <c r="B68" s="95"/>
     </row>
     <row r="69" spans="2:2">
-      <c r="B69" s="106" t="s">
+      <c r="B69" s="96" t="s">
         <v>491</v>
       </c>
     </row>
     <row r="70" spans="2:2">
-      <c r="B70" s="106" t="s">
+      <c r="B70" s="96" t="s">
         <v>492</v>
       </c>
     </row>
     <row r="71" spans="2:2">
-      <c r="B71" s="106" t="s">
+      <c r="B71" s="96" t="s">
         <v>493</v>
       </c>
     </row>
     <row r="72" spans="2:2">
-      <c r="B72" s="106" t="s">
+      <c r="B72" s="96" t="s">
         <v>494</v>
       </c>
     </row>
     <row r="73" spans="2:2">
-      <c r="B73" s="106" t="s">
+      <c r="B73" s="96" t="s">
         <v>495</v>
       </c>
     </row>
     <row r="74" spans="2:2">
-      <c r="B74" s="106" t="s">
+      <c r="B74" s="96" t="s">
         <v>496</v>
       </c>
     </row>
     <row r="75" spans="2:2">
-      <c r="B75" s="106" t="s">
+      <c r="B75" s="96" t="s">
         <v>488</v>
       </c>
     </row>
     <row r="76" spans="2:2">
-      <c r="B76" s="105"/>
+      <c r="B76" s="95"/>
     </row>
     <row r="77" spans="2:2">
-      <c r="B77" s="106" t="s">
+      <c r="B77" s="96" t="s">
         <v>497</v>
       </c>
     </row>
     <row r="78" spans="2:2">
-      <c r="B78" s="106" t="s">
+      <c r="B78" s="96" t="s">
         <v>498</v>
       </c>
     </row>
     <row r="79" spans="2:2">
-      <c r="B79" s="106" t="s">
+      <c r="B79" s="96" t="s">
         <v>499</v>
       </c>
     </row>
     <row r="80" spans="2:2">
-      <c r="B80" s="106" t="s">
+      <c r="B80" s="96" t="s">
         <v>488</v>
       </c>
     </row>
     <row r="81" spans="2:2">
-      <c r="B81" s="105"/>
+      <c r="B81" s="95"/>
     </row>
     <row r="82" spans="2:2">
-      <c r="B82" s="106" t="s">
+      <c r="B82" s="96" t="s">
         <v>500</v>
       </c>
     </row>
     <row r="83" spans="2:2">
-      <c r="B83" s="106" t="s">
+      <c r="B83" s="96" t="s">
         <v>501</v>
       </c>
     </row>
     <row r="84" spans="2:2">
-      <c r="B84" s="106" t="s">
+      <c r="B84" s="96" t="s">
         <v>502</v>
       </c>
     </row>
     <row r="85" spans="2:2">
-      <c r="B85" s="106" t="s">
+      <c r="B85" s="96" t="s">
         <v>503</v>
       </c>
     </row>
     <row r="86" spans="2:2">
-      <c r="B86" s="106" t="s">
+      <c r="B86" s="96" t="s">
         <v>504</v>
       </c>
     </row>
     <row r="87" spans="2:2">
-      <c r="B87" s="106" t="s">
+      <c r="B87" s="96" t="s">
         <v>505</v>
       </c>
     </row>
     <row r="88" spans="2:2">
-      <c r="B88" s="106" t="s">
+      <c r="B88" s="96" t="s">
         <v>488</v>
       </c>
     </row>
     <row r="89" spans="2:2">
-      <c r="B89" s="105"/>
+      <c r="B89" s="95"/>
     </row>
     <row r="90" spans="2:2">
-      <c r="B90" s="107" t="s">
+      <c r="B90" s="97" t="s">
         <v>506</v>
       </c>
     </row>
     <row r="91" spans="2:2">
-      <c r="B91" s="102" t="s">
+      <c r="B91" s="92" t="s">
         <v>532</v>
       </c>
     </row>
     <row r="92" spans="2:2">
-      <c r="B92" s="107" t="s">
+      <c r="B92" s="97" t="s">
         <v>482</v>
       </c>
     </row>
     <row r="93" spans="2:2">
-      <c r="B93" s="107" t="s">
+      <c r="B93" s="97" t="s">
         <v>527</v>
       </c>
     </row>
     <row r="94" spans="2:2">
-      <c r="B94" s="107" t="s">
+      <c r="B94" s="97" t="s">
         <v>528</v>
       </c>
     </row>
     <row r="95" spans="2:2">
-      <c r="B95" s="107" t="s">
+      <c r="B95" s="97" t="s">
         <v>529</v>
       </c>
     </row>
     <row r="96" spans="2:2">
-      <c r="B96" s="107" t="s">
+      <c r="B96" s="97" t="s">
         <v>526</v>
       </c>
     </row>
@@ -14460,132 +14644,132 @@
       </c>
     </row>
     <row r="100" spans="2:2">
-      <c r="B100" s="107" t="s">
+      <c r="B100" s="97" t="s">
         <v>506</v>
       </c>
     </row>
     <row r="101" spans="2:2">
-      <c r="B101" s="107"/>
+      <c r="B101" s="97"/>
     </row>
     <row r="102" spans="2:2">
-      <c r="B102" s="102" t="s">
+      <c r="B102" s="92" t="s">
         <v>507</v>
       </c>
     </row>
     <row r="103" spans="2:2">
-      <c r="B103" s="108" t="s">
+      <c r="B103" s="98" t="s">
         <v>508</v>
       </c>
     </row>
     <row r="104" spans="2:2">
-      <c r="B104" s="108" t="s">
+      <c r="B104" s="98" t="s">
         <v>509</v>
       </c>
     </row>
     <row r="106" spans="2:2">
-      <c r="B106" s="104" t="s">
+      <c r="B106" s="94" t="s">
         <v>510</v>
       </c>
     </row>
     <row r="107" spans="2:2">
-      <c r="B107" s="105"/>
+      <c r="B107" s="95"/>
     </row>
     <row r="108" spans="2:2">
-      <c r="B108" s="106" t="s">
+      <c r="B108" s="96" t="s">
         <v>485</v>
       </c>
     </row>
     <row r="109" spans="2:2">
-      <c r="B109" s="106" t="s">
+      <c r="B109" s="96" t="s">
         <v>511</v>
       </c>
     </row>
     <row r="110" spans="2:2">
-      <c r="B110" s="106" t="s">
+      <c r="B110" s="96" t="s">
         <v>512</v>
       </c>
     </row>
     <row r="111" spans="2:2">
-      <c r="B111" s="106" t="s">
+      <c r="B111" s="96" t="s">
         <v>513</v>
       </c>
     </row>
     <row r="112" spans="2:2">
-      <c r="B112" s="106" t="s">
+      <c r="B112" s="96" t="s">
         <v>533</v>
       </c>
     </row>
     <row r="113" spans="2:2">
-      <c r="B113" s="105"/>
+      <c r="B113" s="95"/>
     </row>
     <row r="114" spans="2:2">
-      <c r="B114" s="106" t="s">
+      <c r="B114" s="96" t="s">
         <v>514</v>
       </c>
     </row>
     <row r="115" spans="2:2">
-      <c r="B115" s="106" t="s">
+      <c r="B115" s="96" t="s">
         <v>515</v>
       </c>
     </row>
     <row r="116" spans="2:2">
-      <c r="B116" s="105"/>
+      <c r="B116" s="95"/>
     </row>
     <row r="117" spans="2:2">
-      <c r="B117" s="106" t="s">
+      <c r="B117" s="96" t="s">
         <v>516</v>
       </c>
     </row>
     <row r="118" spans="2:2">
-      <c r="B118" s="106" t="s">
+      <c r="B118" s="96" t="s">
         <v>517</v>
       </c>
     </row>
     <row r="119" spans="2:2">
-      <c r="B119" s="106" t="s">
+      <c r="B119" s="96" t="s">
         <v>518</v>
       </c>
     </row>
     <row r="120" spans="2:2">
-      <c r="B120" s="106" t="s">
+      <c r="B120" s="96" t="s">
         <v>519</v>
       </c>
     </row>
     <row r="121" spans="2:2">
-      <c r="B121" s="106" t="s">
+      <c r="B121" s="96" t="s">
         <v>520</v>
       </c>
     </row>
     <row r="122" spans="2:2">
-      <c r="B122" s="106" t="s">
+      <c r="B122" s="96" t="s">
         <v>521</v>
       </c>
     </row>
     <row r="123" spans="2:2">
-      <c r="B123" s="106" t="s">
+      <c r="B123" s="96" t="s">
         <v>522</v>
       </c>
     </row>
     <row r="124" spans="2:2">
-      <c r="B124" s="106" t="s">
+      <c r="B124" s="96" t="s">
         <v>523</v>
       </c>
     </row>
     <row r="125" spans="2:2">
-      <c r="B125" s="106" t="s">
+      <c r="B125" s="96" t="s">
         <v>524</v>
       </c>
     </row>
     <row r="126" spans="2:2">
-      <c r="B126" s="106" t="s">
+      <c r="B126" s="96" t="s">
         <v>488</v>
       </c>
     </row>
     <row r="127" spans="2:2">
-      <c r="B127" s="105"/>
+      <c r="B127" s="95"/>
     </row>
     <row r="128" spans="2:2">
-      <c r="B128" s="106" t="s">
+      <c r="B128" s="96" t="s">
         <v>525</v>
       </c>
     </row>
@@ -14710,7 +14894,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B2:C6"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
@@ -14766,4 +14950,51 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="B2:C5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C27" sqref="C27"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="2" max="2" width="60.28515625" customWidth="1"/>
+    <col min="3" max="3" width="89.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:3">
+      <c r="B2" s="38" t="s">
+        <v>46</v>
+      </c>
+      <c r="C2" s="38" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="3" spans="2:3" ht="102.75">
+      <c r="B3" s="109" t="s">
+        <v>534</v>
+      </c>
+      <c r="C3" s="110" t="s">
+        <v>535</v>
+      </c>
+    </row>
+    <row r="4" spans="2:3" ht="30.75">
+      <c r="B4" s="111" t="s">
+        <v>536</v>
+      </c>
+      <c r="C4" s="110" t="s">
+        <v>537</v>
+      </c>
+    </row>
+    <row r="5" spans="2:3">
+      <c r="B5" s="1"/>
+      <c r="C5" s="40"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
some changes on Training plan
</commit_message>
<xml_diff>
--- a/Training_Plan.xlsx
+++ b/Training_Plan.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="45" windowWidth="19155" windowHeight="8400" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="45" windowWidth="18990" windowHeight="7800" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Plan" sheetId="1" r:id="rId1"/>
@@ -15,6 +15,8 @@
     <sheet name="MongoDBJasper" sheetId="6" r:id="rId6"/>
     <sheet name="JUNIT" sheetId="7" r:id="rId7"/>
     <sheet name="Logging" sheetId="8" r:id="rId8"/>
+    <sheet name="AngularJS" sheetId="12" r:id="rId9"/>
+    <sheet name="NodeJS" sheetId="10" r:id="rId10"/>
   </sheets>
   <definedNames>
     <definedName name="jaxrs_intro" localSheetId="3">'RESTful WS'!$B$6</definedName>
@@ -24,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="677" uniqueCount="619">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="718" uniqueCount="656">
   <si>
     <t>Java core</t>
   </si>
@@ -13186,12 +13188,661 @@
   <si>
     <t>http://www.basilv.com/psd/blog/2009/java-based-configuration-of-spring-dependency-injection</t>
   </si>
+  <si>
+    <t>What is Node.js?</t>
+  </si>
+  <si>
+    <t>Features of Node.js</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"># </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Node.js is a platform built on Chrome's JavaScript runtime for easily building fast and scalable network applications
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"># </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Node.js is an open source, cross-platform runtime environment for developing server-side and networking applications
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"># </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Node.js also provides a rich library of various JavaScript modules which simplifies the development of web applications using Node.js to a great extent
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Node.js = Runtime Environment + JavaScript Library</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t># Asynchronous and Event Driven</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> All APIs of Node.js library are asynchronous that is, non-blocking
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"># Very Fast </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Being built on Google Chrome's V8 JavaScript Engine, Node.js library is very fast in code execution.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t># Single Threaded but Highly Scalable</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> - Node.js uses a single threaded model with event looping. Event mechanism helps the server to respond in a non-blocking way and makes the server highly scalable as opposed to traditional servers which create limited threads to handle requests.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t># No Buffering</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> - Node.js applications never buffer any data. These applications simply output the data in chunks</t>
+    </r>
+  </si>
+  <si>
+    <t>Concepts</t>
+  </si>
+  <si>
+    <t>The following diagram depicts some important parts of Node.js which we will discuss in detail in the subsequent chapters.</t>
+  </si>
+  <si>
+    <t>Where to Use Node.js?</t>
+  </si>
+  <si>
+    <t># I/O bound Applications
+# Data Streaming Applications
+# Data Intensive Real time Applications (DIRT)
+# JSON APIs based Applications
+# Single Page Applications</t>
+  </si>
+  <si>
+    <t>AngularJS Introduction</t>
+  </si>
+  <si>
+    <t># AngularJS is a JavaScript framework. It can be added to an HTML page with a &lt;script&gt; tag.
+# AngularJS extends HTML attributes with Directives, and binds data to HTML with Expressions.</t>
+  </si>
+  <si>
+    <t>AngularJS Expressions</t>
+  </si>
+  <si>
+    <t># AngularJS expressions are written inside double braces: {{ expression }}.
+# AngularJS expressions binds data to HTML the same way as the ng-bind directive.
+# AngularJS expressions are much like JavaScript expressions: They can contain literals, operators, and variables.</t>
+  </si>
+  <si>
+    <t>AngularJS Expressions vs. JavaScript Expressions</t>
+  </si>
+  <si>
+    <t># Like JavaScript expressions, AngularJS expressions can contain literals, operators, and variables.</t>
+  </si>
+  <si>
+    <t># Unlike JavaScript expressions, AngularJS expressions can be written inside HTML.</t>
+  </si>
+  <si>
+    <t># AngularJS expressions do not support conditionals, loops, and exceptions, while JavaScript expressions do.</t>
+  </si>
+  <si>
+    <t># AngularJS expressions support filters, while JavaScript expressions do not.</t>
+  </si>
+  <si>
+    <t>AngularJS Directives</t>
+  </si>
+  <si>
+    <t># AngularJS lets you extend HTML with new attributes called Directives.
+# AngularJS directives are extended HTML attributes with the prefix ng-.</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">&lt;div </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>ng-app</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>="" ng-init="firstName='John'"&gt;
+&lt;p&gt;Name: &lt;input type="text" ng-model="firstName"&gt;&lt;/p&gt;
+&lt;p&gt;You wrote: {{ firstName }}&lt;/p&gt;
+&lt;/div&gt;</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>The </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Verdana"/>
+        <family val="2"/>
+      </rPr>
+      <t>ng-init</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Verdana"/>
+        <family val="2"/>
+      </rPr>
+      <t> directive initializes application data.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>The </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Verdana"/>
+        <family val="2"/>
+      </rPr>
+      <t>ng-app</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Verdana"/>
+        <family val="2"/>
+      </rPr>
+      <t> directive initializes an AngularJS application.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>The </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Verdana"/>
+        <family val="2"/>
+      </rPr>
+      <t>ng-model</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Verdana"/>
+        <family val="2"/>
+      </rPr>
+      <t> directive binds the value of HTML controls (input, select, textarea) to application data.</t>
+    </r>
+  </si>
+  <si>
+    <t>Repeating HTML Elements</t>
+  </si>
+  <si>
+    <t>The ng-repeat directive repeats an HTML element:
+&lt;div ng-app="" ng-init="names=['Jani','Hege','Kai']"&gt;
+  &lt;ul&gt;
+    &lt;li ng-repeat="x in names"&gt;
+      {{ x }}
+    &lt;/li&gt;
+  &lt;/ul&gt;
+&lt;/div&gt;</t>
+  </si>
+  <si>
+    <t>AngularJS Controllers</t>
+  </si>
+  <si>
+    <t># AngularJS controllers control the data of AngularJS applications.
+# AngularJS controllers are regular JavaScript Objects.
+# The ng-controller directive defines the application controller.</t>
+  </si>
+  <si>
+    <t>S.O.L.I.D Concepts</t>
+  </si>
+  <si>
+    <r>
+      <t>S</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="15"/>
+        <color rgb="FF333333"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t> – Single-responsiblity principle</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>O</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="15"/>
+        <color rgb="FF333333"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t> – Open-closed principle</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>L</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="15"/>
+        <color rgb="FF333333"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t> – Liskov substitution principle</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>I</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="15"/>
+        <color rgb="FF333333"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t> – Interface segregation principle</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>D</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="15"/>
+        <color rgb="FF333333"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t> – Dependency Inversion Principle</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>A class should have one and only one reason to change, meaning that a class should have only one job.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+Ex: say we have some shapes and we want to sum all the areas of the shapes.
+- </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Shape</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> class: contains the information of shape
+- </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>AreaCalculator</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> class is responsible for calculating the sum of all areas
+- </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>SumCalculatorOutputter</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> class is responsible for displaying the result of AreaCalculator</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Objects or entities should be open for extension, but closed for modification.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>public function sum() {</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+   foreach($this-&gt;shapes as $shape) {
+        if(is_a($shape, 'Square')) {
+            $area[] = pow($shape-&gt;length, 2);
+        } else if(is_a($shape, 'Circle')) {
+            $area[] = pi() * pow($shape-&gt;radius, 2);
+        }
+    }
+    return array_sum($area);
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">}   
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">If we wanted the sum method to be able to sum the areas of more shapes, we would have to add more if/else blocks and that goes against the Open-closed principle.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>SOLUTION: Strategy pattern</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+public function sum() {
+    foreach($this-&gt;shapes as $ShapeInterface) {
+        $area[] = $shape-&gt;area;
+    }
+    return array_sum($area);
+}</t>
+    </r>
+  </si>
+  <si>
+    <t>Child classes should never break the parent class' type definitions.
+Liskovs Substitution Principle states that any method that takes class X as a parameter must be able to work with any subclasses of X.</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Clients should not be forced to implement unnecessary methods which they will not use</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+Take an example. Developer Alex created an interface Reportable and added two methods generateExcel() and generatedPdf(). Now client ‘A’ wants to use this interface but he intend to use reports only in PDF format and not in excel. Will he achieve the functionality easily.
+NO. He will have to implement two methods, out of which one is extra burden put on him by designer of software. Either he will implement another method or leave it blank. So are not desired cases, right??
+So what is the solution? Solution is to create two interfaces by breaking the existing one. They should be like PdfReportable and ExcelReportable. This will give the flexibility to user to use only required functionality only.</t>
+    </r>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="57">
+  <fonts count="67">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -13574,6 +14225,71 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="18.7"/>
+      <color rgb="FF121214"/>
+      <name val="Verdana"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Verdana"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="27"/>
+      <color rgb="FF000000"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="20"/>
+      <color rgb="FF000000"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="23"/>
+      <color rgb="FF000000"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Verdana"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color rgb="FF545454"/>
+      <name val="Open Sans"/>
+    </font>
+    <font>
+      <sz val="15"/>
+      <color rgb="FF333333"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color rgb="FF333333"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <i/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="5">
     <fill>
@@ -13601,7 +14317,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="15">
+  <borders count="16">
     <border>
       <left/>
       <right/>
@@ -13785,6 +14501,19 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="0" tint="-0.499984740745262"/>
+      </right>
+      <top style="thin">
+        <color theme="0" tint="-0.499984740745262"/>
+      </top>
+      <bottom style="thin">
+        <color theme="0" tint="-0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -13793,7 +14522,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="125">
+  <cellXfs count="137">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -14077,6 +14806,9 @@
     <xf numFmtId="0" fontId="56" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
@@ -14107,6 +14839,33 @@
     <xf numFmtId="0" fontId="20" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="57" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="58" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="60" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="61" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="59" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="58" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="61" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="63" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="65" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -14128,13 +14887,13 @@
     <xdr:from>
       <xdr:col>4</xdr:col>
       <xdr:colOff>47624</xdr:colOff>
-      <xdr:row>89</xdr:row>
+      <xdr:row>95</xdr:row>
       <xdr:rowOff>28575</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
       <xdr:colOff>85724</xdr:colOff>
-      <xdr:row>99</xdr:row>
+      <xdr:row>105</xdr:row>
       <xdr:rowOff>95250</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -14172,13 +14931,13 @@
     <xdr:from>
       <xdr:col>2</xdr:col>
       <xdr:colOff>752475</xdr:colOff>
-      <xdr:row>141</xdr:row>
+      <xdr:row>147</xdr:row>
       <xdr:rowOff>76200</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
       <xdr:colOff>3019425</xdr:colOff>
-      <xdr:row>180</xdr:row>
+      <xdr:row>186</xdr:row>
       <xdr:rowOff>114300</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -14380,6 +15139,51 @@
         <a:xfrm>
           <a:off x="1190625" y="35204400"/>
           <a:ext cx="7981950" cy="1162050"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>180975</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>266700</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>3790950</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>3276600</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3073" name="Picture 1" descr="Node.js Concepts"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print"/>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="4181475" y="3914775"/>
+          <a:ext cx="3609975" cy="3009900"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -15141,12 +15945,470 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="B2:C128"/>
+  <sheetViews>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="5.140625" customWidth="1"/>
+    <col min="2" max="2" width="54.85546875" customWidth="1"/>
+    <col min="3" max="3" width="107.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:3">
+      <c r="B2" s="38" t="s">
+        <v>46</v>
+      </c>
+      <c r="C2" s="38" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="3" spans="2:3" ht="105">
+      <c r="B3" s="126" t="s">
+        <v>619</v>
+      </c>
+      <c r="C3" s="39" t="s">
+        <v>621</v>
+      </c>
+    </row>
+    <row r="4" spans="2:3" ht="91.5">
+      <c r="B4" s="126" t="s">
+        <v>620</v>
+      </c>
+      <c r="C4" s="127" t="s">
+        <v>622</v>
+      </c>
+    </row>
+    <row r="5" spans="2:3" ht="30.75">
+      <c r="B5" s="126" t="s">
+        <v>623</v>
+      </c>
+      <c r="C5" s="127" t="s">
+        <v>624</v>
+      </c>
+    </row>
+    <row r="6" spans="2:3" ht="267.75" customHeight="1">
+      <c r="B6" s="4"/>
+      <c r="C6" s="2"/>
+    </row>
+    <row r="7" spans="2:3" ht="76.5">
+      <c r="B7" s="126" t="s">
+        <v>625</v>
+      </c>
+      <c r="C7" s="115" t="s">
+        <v>626</v>
+      </c>
+    </row>
+    <row r="8" spans="2:3">
+      <c r="B8" s="2"/>
+      <c r="C8" s="115"/>
+    </row>
+    <row r="9" spans="2:3">
+      <c r="B9" s="15"/>
+      <c r="C9" s="15"/>
+    </row>
+    <row r="10" spans="2:3">
+      <c r="B10" s="115"/>
+      <c r="C10" s="2"/>
+    </row>
+    <row r="11" spans="2:3">
+      <c r="B11" s="115"/>
+      <c r="C11" s="2"/>
+    </row>
+    <row r="12" spans="2:3">
+      <c r="B12" s="115"/>
+      <c r="C12" s="2"/>
+    </row>
+    <row r="13" spans="2:3">
+      <c r="B13" s="115"/>
+      <c r="C13" s="2"/>
+    </row>
+    <row r="14" spans="2:3">
+      <c r="B14" s="115"/>
+      <c r="C14" s="2"/>
+    </row>
+    <row r="15" spans="2:3">
+      <c r="B15" s="115"/>
+      <c r="C15" s="2"/>
+    </row>
+    <row r="16" spans="2:3">
+      <c r="B16" s="115"/>
+      <c r="C16" s="2"/>
+    </row>
+    <row r="17" spans="2:3">
+      <c r="B17" s="2"/>
+      <c r="C17" s="115"/>
+    </row>
+    <row r="18" spans="2:3">
+      <c r="B18" s="2"/>
+      <c r="C18" s="41"/>
+    </row>
+    <row r="19" spans="2:3">
+      <c r="B19" s="4"/>
+      <c r="C19" s="42"/>
+    </row>
+    <row r="20" spans="2:3">
+      <c r="B20" s="2"/>
+      <c r="C20" s="115"/>
+    </row>
+    <row r="21" spans="2:3" ht="409.5" customHeight="1">
+      <c r="B21" s="2"/>
+      <c r="C21" s="40"/>
+    </row>
+    <row r="22" spans="2:3">
+      <c r="B22" s="2"/>
+      <c r="C22" s="115"/>
+    </row>
+    <row r="23" spans="2:3">
+      <c r="B23" s="2"/>
+      <c r="C23" s="115"/>
+    </row>
+    <row r="24" spans="2:3">
+      <c r="B24" s="43"/>
+      <c r="C24" s="40"/>
+    </row>
+    <row r="25" spans="2:3">
+      <c r="B25" s="43"/>
+      <c r="C25" s="40"/>
+    </row>
+    <row r="26" spans="2:3" ht="26.25">
+      <c r="B26" s="44"/>
+      <c r="C26" s="115"/>
+    </row>
+    <row r="27" spans="2:3" ht="33" customHeight="1">
+      <c r="B27" s="125"/>
+      <c r="C27" s="125"/>
+    </row>
+    <row r="28" spans="2:3">
+      <c r="B28" s="125"/>
+      <c r="C28" s="125"/>
+    </row>
+    <row r="29" spans="2:3" ht="15.75" thickBot="1">
+      <c r="B29" s="48"/>
+      <c r="C29" s="49"/>
+    </row>
+    <row r="30" spans="2:3" ht="15.75" thickBot="1">
+      <c r="B30" s="47"/>
+      <c r="C30" s="2"/>
+    </row>
+    <row r="31" spans="2:3" ht="15.75" thickBot="1">
+      <c r="B31" s="46"/>
+      <c r="C31" s="2"/>
+    </row>
+    <row r="32" spans="2:3" ht="15.75" thickBot="1">
+      <c r="B32" s="47"/>
+      <c r="C32" s="2"/>
+    </row>
+    <row r="33" spans="2:3" ht="15.75" thickBot="1">
+      <c r="B33" s="45"/>
+      <c r="C33" s="2"/>
+    </row>
+    <row r="34" spans="2:3" ht="15.75" thickBot="1">
+      <c r="B34" s="47"/>
+      <c r="C34" s="2"/>
+    </row>
+    <row r="35" spans="2:3" ht="15.75" thickBot="1">
+      <c r="B35" s="46"/>
+      <c r="C35" s="2"/>
+    </row>
+    <row r="36" spans="2:3" ht="15.75" thickBot="1">
+      <c r="B36" s="46"/>
+      <c r="C36" s="2"/>
+    </row>
+    <row r="37" spans="2:3">
+      <c r="B37" s="50"/>
+      <c r="C37" s="51"/>
+    </row>
+    <row r="38" spans="2:3" ht="50.25" customHeight="1">
+      <c r="B38" s="125"/>
+      <c r="C38" s="125"/>
+    </row>
+    <row r="39" spans="2:3" ht="32.25" customHeight="1">
+      <c r="B39" s="125"/>
+      <c r="C39" s="125"/>
+    </row>
+    <row r="40" spans="2:3" ht="15.75" thickBot="1">
+      <c r="B40" s="52"/>
+      <c r="C40" s="49"/>
+    </row>
+    <row r="41" spans="2:3" ht="15.75" thickBot="1">
+      <c r="B41" s="46"/>
+      <c r="C41" s="2"/>
+    </row>
+    <row r="42" spans="2:3" ht="15.75" thickBot="1">
+      <c r="B42" s="46"/>
+    </row>
+    <row r="43" spans="2:3" ht="15.75" thickBot="1">
+      <c r="B43" s="46"/>
+    </row>
+    <row r="44" spans="2:3" ht="15.75" thickBot="1">
+      <c r="B44" s="46"/>
+    </row>
+    <row r="45" spans="2:3" ht="15.75" thickBot="1">
+      <c r="B45" s="46"/>
+    </row>
+    <row r="46" spans="2:3" ht="15.75" thickBot="1">
+      <c r="B46" s="46"/>
+    </row>
+    <row r="47" spans="2:3" ht="15.75" thickBot="1">
+      <c r="B47" s="46"/>
+    </row>
+    <row r="48" spans="2:3">
+      <c r="B48" s="50"/>
+    </row>
+    <row r="49" spans="2:3" ht="36" customHeight="1">
+      <c r="B49" s="125"/>
+      <c r="C49" s="125"/>
+    </row>
+    <row r="50" spans="2:3" ht="49.5" customHeight="1">
+      <c r="B50" s="125"/>
+      <c r="C50" s="125"/>
+    </row>
+    <row r="52" spans="2:3" ht="41.25">
+      <c r="B52" s="91"/>
+    </row>
+    <row r="53" spans="2:3">
+      <c r="B53" s="92"/>
+    </row>
+    <row r="54" spans="2:3">
+      <c r="B54" s="93"/>
+    </row>
+    <row r="55" spans="2:3">
+      <c r="B55" s="93"/>
+    </row>
+    <row r="56" spans="2:3">
+      <c r="B56" s="93"/>
+    </row>
+    <row r="57" spans="2:3">
+      <c r="B57" s="94"/>
+    </row>
+    <row r="58" spans="2:3">
+      <c r="B58" s="95"/>
+    </row>
+    <row r="59" spans="2:3">
+      <c r="B59" s="96"/>
+    </row>
+    <row r="60" spans="2:3">
+      <c r="B60" s="96"/>
+    </row>
+    <row r="61" spans="2:3">
+      <c r="B61" s="96"/>
+    </row>
+    <row r="62" spans="2:3">
+      <c r="B62" s="96"/>
+    </row>
+    <row r="63" spans="2:3">
+      <c r="B63" s="95"/>
+    </row>
+    <row r="64" spans="2:3">
+      <c r="B64" s="96"/>
+    </row>
+    <row r="65" spans="2:2">
+      <c r="B65" s="96"/>
+    </row>
+    <row r="66" spans="2:2">
+      <c r="B66" s="96"/>
+    </row>
+    <row r="67" spans="2:2">
+      <c r="B67" s="96"/>
+    </row>
+    <row r="68" spans="2:2">
+      <c r="B68" s="95"/>
+    </row>
+    <row r="69" spans="2:2">
+      <c r="B69" s="96"/>
+    </row>
+    <row r="70" spans="2:2">
+      <c r="B70" s="96"/>
+    </row>
+    <row r="71" spans="2:2">
+      <c r="B71" s="96"/>
+    </row>
+    <row r="72" spans="2:2">
+      <c r="B72" s="96"/>
+    </row>
+    <row r="73" spans="2:2">
+      <c r="B73" s="96"/>
+    </row>
+    <row r="74" spans="2:2">
+      <c r="B74" s="96"/>
+    </row>
+    <row r="75" spans="2:2">
+      <c r="B75" s="96"/>
+    </row>
+    <row r="76" spans="2:2">
+      <c r="B76" s="95"/>
+    </row>
+    <row r="77" spans="2:2">
+      <c r="B77" s="96"/>
+    </row>
+    <row r="78" spans="2:2">
+      <c r="B78" s="96"/>
+    </row>
+    <row r="79" spans="2:2">
+      <c r="B79" s="96"/>
+    </row>
+    <row r="80" spans="2:2">
+      <c r="B80" s="96"/>
+    </row>
+    <row r="81" spans="2:2">
+      <c r="B81" s="95"/>
+    </row>
+    <row r="82" spans="2:2">
+      <c r="B82" s="96"/>
+    </row>
+    <row r="83" spans="2:2">
+      <c r="B83" s="96"/>
+    </row>
+    <row r="84" spans="2:2">
+      <c r="B84" s="96"/>
+    </row>
+    <row r="85" spans="2:2">
+      <c r="B85" s="96"/>
+    </row>
+    <row r="86" spans="2:2">
+      <c r="B86" s="96"/>
+    </row>
+    <row r="87" spans="2:2">
+      <c r="B87" s="96"/>
+    </row>
+    <row r="88" spans="2:2">
+      <c r="B88" s="96"/>
+    </row>
+    <row r="89" spans="2:2">
+      <c r="B89" s="95"/>
+    </row>
+    <row r="90" spans="2:2">
+      <c r="B90" s="97"/>
+    </row>
+    <row r="91" spans="2:2">
+      <c r="B91" s="92"/>
+    </row>
+    <row r="92" spans="2:2">
+      <c r="B92" s="97"/>
+    </row>
+    <row r="93" spans="2:2">
+      <c r="B93" s="97"/>
+    </row>
+    <row r="94" spans="2:2">
+      <c r="B94" s="97"/>
+    </row>
+    <row r="95" spans="2:2">
+      <c r="B95" s="97"/>
+    </row>
+    <row r="96" spans="2:2">
+      <c r="B96" s="97"/>
+    </row>
+    <row r="100" spans="2:2">
+      <c r="B100" s="97"/>
+    </row>
+    <row r="101" spans="2:2">
+      <c r="B101" s="97"/>
+    </row>
+    <row r="102" spans="2:2">
+      <c r="B102" s="92"/>
+    </row>
+    <row r="103" spans="2:2">
+      <c r="B103" s="98"/>
+    </row>
+    <row r="104" spans="2:2">
+      <c r="B104" s="98"/>
+    </row>
+    <row r="106" spans="2:2">
+      <c r="B106" s="94"/>
+    </row>
+    <row r="107" spans="2:2">
+      <c r="B107" s="95"/>
+    </row>
+    <row r="108" spans="2:2">
+      <c r="B108" s="96"/>
+    </row>
+    <row r="109" spans="2:2">
+      <c r="B109" s="96"/>
+    </row>
+    <row r="110" spans="2:2">
+      <c r="B110" s="96"/>
+    </row>
+    <row r="111" spans="2:2">
+      <c r="B111" s="96"/>
+    </row>
+    <row r="112" spans="2:2">
+      <c r="B112" s="96"/>
+    </row>
+    <row r="113" spans="2:2">
+      <c r="B113" s="95"/>
+    </row>
+    <row r="114" spans="2:2">
+      <c r="B114" s="96"/>
+    </row>
+    <row r="115" spans="2:2">
+      <c r="B115" s="96"/>
+    </row>
+    <row r="116" spans="2:2">
+      <c r="B116" s="95"/>
+    </row>
+    <row r="117" spans="2:2">
+      <c r="B117" s="96"/>
+    </row>
+    <row r="118" spans="2:2">
+      <c r="B118" s="96"/>
+    </row>
+    <row r="119" spans="2:2">
+      <c r="B119" s="96"/>
+    </row>
+    <row r="120" spans="2:2">
+      <c r="B120" s="96"/>
+    </row>
+    <row r="121" spans="2:2">
+      <c r="B121" s="96"/>
+    </row>
+    <row r="122" spans="2:2">
+      <c r="B122" s="96"/>
+    </row>
+    <row r="123" spans="2:2">
+      <c r="B123" s="96"/>
+    </row>
+    <row r="124" spans="2:2">
+      <c r="B124" s="96"/>
+    </row>
+    <row r="125" spans="2:2">
+      <c r="B125" s="96"/>
+    </row>
+    <row r="126" spans="2:2">
+      <c r="B126" s="96"/>
+    </row>
+    <row r="127" spans="2:2">
+      <c r="B127" s="95"/>
+    </row>
+    <row r="128" spans="2:2">
+      <c r="B128" s="96"/>
+    </row>
+  </sheetData>
+  <mergeCells count="6">
+    <mergeCell ref="B27:C27"/>
+    <mergeCell ref="B28:C28"/>
+    <mergeCell ref="B38:C38"/>
+    <mergeCell ref="B39:C39"/>
+    <mergeCell ref="B49:C49"/>
+    <mergeCell ref="B50:C50"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B2:E197"/>
+  <dimension ref="B2:E203"/>
   <sheetViews>
-    <sheetView topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="D51" sqref="D51"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -15226,1101 +16488,1109 @@
       <c r="D8" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="E8" s="14" t="s">
+      <c r="E8" s="115" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="9" spans="2:5">
-      <c r="B9" s="23"/>
-      <c r="C9" s="23"/>
-      <c r="D9" s="23"/>
-      <c r="E9" s="24"/>
-    </row>
-    <row r="10" spans="2:5" ht="31.5">
-      <c r="B10" s="22" t="s">
-        <v>101</v>
-      </c>
-      <c r="C10" s="23"/>
-      <c r="D10" s="23"/>
-      <c r="E10" s="24"/>
-    </row>
-    <row r="12" spans="2:5">
-      <c r="B12" s="19" t="s">
-        <v>3</v>
-      </c>
-      <c r="C12" s="19"/>
-      <c r="D12" s="19" t="s">
-        <v>46</v>
-      </c>
-      <c r="E12" s="19" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="13" spans="2:5" ht="18.75">
-      <c r="B13" s="2">
-        <v>1</v>
-      </c>
-      <c r="C13" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="D13" s="18" t="s">
-        <v>58</v>
-      </c>
-      <c r="E13" s="2"/>
-    </row>
-    <row r="14" spans="2:5">
+    <row r="9" spans="2:5" ht="23.25">
+      <c r="B9" s="135" t="s">
+        <v>646</v>
+      </c>
+      <c r="C9" s="2"/>
+      <c r="D9" s="2"/>
+      <c r="E9" s="115"/>
+    </row>
+    <row r="10" spans="2:5" ht="105">
+      <c r="B10" s="2"/>
+      <c r="C10" s="2"/>
+      <c r="D10" s="136" t="s">
+        <v>647</v>
+      </c>
+      <c r="E10" s="115" t="s">
+        <v>652</v>
+      </c>
+    </row>
+    <row r="11" spans="2:5" ht="315">
+      <c r="B11" s="2"/>
+      <c r="C11" s="2"/>
+      <c r="D11" s="136" t="s">
+        <v>648</v>
+      </c>
+      <c r="E11" s="115" t="s">
+        <v>653</v>
+      </c>
+    </row>
+    <row r="12" spans="2:5" ht="45">
+      <c r="B12" s="2"/>
+      <c r="C12" s="2"/>
+      <c r="D12" s="136" t="s">
+        <v>649</v>
+      </c>
+      <c r="E12" s="115" t="s">
+        <v>654</v>
+      </c>
+    </row>
+    <row r="13" spans="2:5" ht="210">
+      <c r="B13" s="2"/>
+      <c r="C13" s="2"/>
+      <c r="D13" s="136" t="s">
+        <v>650</v>
+      </c>
+      <c r="E13" s="115" t="s">
+        <v>655</v>
+      </c>
+    </row>
+    <row r="14" spans="2:5" ht="19.5">
       <c r="B14" s="2"/>
       <c r="C14" s="2"/>
-      <c r="D14" s="115" t="s">
-        <v>47</v>
-      </c>
-      <c r="E14" s="116"/>
+      <c r="D14" s="136" t="s">
+        <v>651</v>
+      </c>
+      <c r="E14" s="115"/>
     </row>
     <row r="15" spans="2:5">
-      <c r="B15" s="2"/>
-      <c r="C15" s="2"/>
-      <c r="D15" s="15" t="s">
-        <v>48</v>
-      </c>
-      <c r="E15" s="15" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="16" spans="2:5">
-      <c r="B16" s="2"/>
-      <c r="C16" s="2"/>
-      <c r="D16" s="16" t="s">
-        <v>50</v>
-      </c>
-      <c r="E16" s="16" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="17" spans="2:5" ht="45">
-      <c r="B17" s="2"/>
-      <c r="C17" s="2"/>
-      <c r="D17" s="16" t="s">
-        <v>52</v>
-      </c>
-      <c r="E17" s="16" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="18" spans="2:5" ht="30">
-      <c r="B18" s="2"/>
-      <c r="C18" s="2"/>
-      <c r="D18" s="16" t="s">
-        <v>54</v>
-      </c>
-      <c r="E18" s="16" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="19" spans="2:5">
-      <c r="B19" s="2"/>
-      <c r="C19" s="2"/>
-      <c r="D19" s="16" t="s">
-        <v>56</v>
-      </c>
-      <c r="E19" s="16" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="20" spans="2:5" ht="18.75">
+      <c r="B15" s="23"/>
+      <c r="C15" s="23"/>
+      <c r="D15" s="23"/>
+      <c r="E15" s="24"/>
+    </row>
+    <row r="16" spans="2:5" ht="31.5">
+      <c r="B16" s="22" t="s">
+        <v>101</v>
+      </c>
+      <c r="C16" s="23"/>
+      <c r="D16" s="23"/>
+      <c r="E16" s="24"/>
+    </row>
+    <row r="18" spans="2:5">
+      <c r="B18" s="19" t="s">
+        <v>3</v>
+      </c>
+      <c r="C18" s="19"/>
+      <c r="D18" s="19" t="s">
+        <v>46</v>
+      </c>
+      <c r="E18" s="19" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="19" spans="2:5" ht="18.75">
+      <c r="B19" s="2">
+        <v>1</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D19" s="18" t="s">
+        <v>58</v>
+      </c>
+      <c r="E19" s="2"/>
+    </row>
+    <row r="20" spans="2:5">
       <c r="B20" s="2"/>
       <c r="C20" s="2"/>
-      <c r="D20" s="18" t="s">
-        <v>77</v>
-      </c>
-      <c r="E20" s="16"/>
+      <c r="D20" s="116" t="s">
+        <v>47</v>
+      </c>
+      <c r="E20" s="117"/>
     </row>
     <row r="21" spans="2:5">
       <c r="B21" s="2"/>
       <c r="C21" s="2"/>
-      <c r="D21" s="119" t="s">
-        <v>78</v>
-      </c>
-      <c r="E21" s="119"/>
+      <c r="D21" s="15" t="s">
+        <v>48</v>
+      </c>
+      <c r="E21" s="15" t="s">
+        <v>49</v>
+      </c>
     </row>
     <row r="22" spans="2:5">
       <c r="B22" s="2"/>
       <c r="C22" s="2"/>
-      <c r="D22" s="15" t="s">
-        <v>48</v>
-      </c>
-      <c r="E22" s="15" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="23" spans="2:5">
+      <c r="D22" s="16" t="s">
+        <v>50</v>
+      </c>
+      <c r="E22" s="16" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="23" spans="2:5" ht="45">
       <c r="B23" s="2"/>
       <c r="C23" s="2"/>
-      <c r="D23" s="14" t="s">
-        <v>80</v>
-      </c>
-      <c r="E23" s="14" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="24" spans="2:5" ht="45">
+      <c r="D23" s="16" t="s">
+        <v>52</v>
+      </c>
+      <c r="E23" s="16" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="24" spans="2:5" ht="30">
       <c r="B24" s="2"/>
       <c r="C24" s="2"/>
-      <c r="D24" s="74" t="s">
-        <v>420</v>
-      </c>
-      <c r="E24" s="14" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="25" spans="2:5" ht="30">
+      <c r="D24" s="16" t="s">
+        <v>54</v>
+      </c>
+      <c r="E24" s="16" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="25" spans="2:5">
       <c r="B25" s="2"/>
       <c r="C25" s="2"/>
-      <c r="D25" s="74" t="s">
-        <v>421</v>
-      </c>
-      <c r="E25" s="14" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="26" spans="2:5" ht="30">
+      <c r="D25" s="16" t="s">
+        <v>56</v>
+      </c>
+      <c r="E25" s="16" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="26" spans="2:5" ht="18.75">
       <c r="B26" s="2"/>
       <c r="C26" s="2"/>
-      <c r="D26" s="74" t="s">
-        <v>422</v>
-      </c>
-      <c r="E26" s="14" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="27" spans="2:5" ht="18.75">
+      <c r="D26" s="18" t="s">
+        <v>77</v>
+      </c>
+      <c r="E26" s="16"/>
+    </row>
+    <row r="27" spans="2:5">
       <c r="B27" s="2"/>
       <c r="C27" s="2"/>
-      <c r="D27" s="20" t="s">
-        <v>85</v>
-      </c>
-      <c r="E27" s="20"/>
+      <c r="D27" s="120" t="s">
+        <v>78</v>
+      </c>
+      <c r="E27" s="120"/>
     </row>
     <row r="28" spans="2:5">
       <c r="B28" s="2"/>
       <c r="C28" s="2"/>
-      <c r="D28" s="120" t="s">
-        <v>86</v>
-      </c>
-      <c r="E28" s="121"/>
+      <c r="D28" s="15" t="s">
+        <v>48</v>
+      </c>
+      <c r="E28" s="15" t="s">
+        <v>79</v>
+      </c>
     </row>
     <row r="29" spans="2:5">
       <c r="B29" s="2"/>
       <c r="C29" s="2"/>
-      <c r="D29" s="15" t="s">
-        <v>87</v>
-      </c>
-      <c r="E29" s="15" t="s">
-        <v>88</v>
+      <c r="D29" s="14" t="s">
+        <v>80</v>
+      </c>
+      <c r="E29" s="14" t="s">
+        <v>81</v>
       </c>
     </row>
     <row r="30" spans="2:5" ht="45">
       <c r="B30" s="2"/>
       <c r="C30" s="2"/>
-      <c r="D30" s="14" t="s">
-        <v>89</v>
+      <c r="D30" s="74" t="s">
+        <v>420</v>
       </c>
       <c r="E30" s="14" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="31" spans="2:5">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="31" spans="2:5" ht="30">
       <c r="B31" s="2"/>
       <c r="C31" s="2"/>
-      <c r="D31" s="14" t="s">
-        <v>91</v>
+      <c r="D31" s="74" t="s">
+        <v>421</v>
       </c>
       <c r="E31" s="14" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="32" spans="2:5">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="32" spans="2:5" ht="30">
       <c r="B32" s="2"/>
       <c r="C32" s="2"/>
-      <c r="D32" s="14" t="s">
-        <v>93</v>
+      <c r="D32" s="74" t="s">
+        <v>422</v>
       </c>
       <c r="E32" s="14" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="33" spans="2:5">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="33" spans="2:5" ht="18.75">
       <c r="B33" s="2"/>
       <c r="C33" s="2"/>
-      <c r="D33" s="14" t="s">
-        <v>95</v>
-      </c>
-      <c r="E33" s="14" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="34" spans="2:5" ht="30">
+      <c r="D33" s="20" t="s">
+        <v>85</v>
+      </c>
+      <c r="E33" s="20"/>
+    </row>
+    <row r="34" spans="2:5">
       <c r="B34" s="2"/>
       <c r="C34" s="2"/>
-      <c r="D34" s="14" t="s">
-        <v>97</v>
-      </c>
-      <c r="E34" s="14" t="s">
-        <v>98</v>
-      </c>
+      <c r="D34" s="121" t="s">
+        <v>86</v>
+      </c>
+      <c r="E34" s="122"/>
     </row>
     <row r="35" spans="2:5">
-      <c r="B35" s="2">
-        <v>2</v>
-      </c>
-      <c r="C35" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="D35" s="2"/>
-      <c r="E35" s="2"/>
-    </row>
-    <row r="36" spans="2:5" ht="18.75">
-      <c r="B36" s="2">
-        <v>3</v>
-      </c>
-      <c r="C36" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="D36" s="18" t="s">
-        <v>59</v>
-      </c>
-      <c r="E36" s="2"/>
+      <c r="B35" s="2"/>
+      <c r="C35" s="2"/>
+      <c r="D35" s="15" t="s">
+        <v>87</v>
+      </c>
+      <c r="E35" s="15" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="36" spans="2:5" ht="45">
+      <c r="B36" s="2"/>
+      <c r="C36" s="2"/>
+      <c r="D36" s="14" t="s">
+        <v>89</v>
+      </c>
+      <c r="E36" s="14" t="s">
+        <v>90</v>
+      </c>
     </row>
     <row r="37" spans="2:5">
       <c r="B37" s="2"/>
       <c r="C37" s="2"/>
-      <c r="D37" s="117" t="s">
-        <v>60</v>
-      </c>
-      <c r="E37" s="117"/>
+      <c r="D37" s="14" t="s">
+        <v>91</v>
+      </c>
+      <c r="E37" s="14" t="s">
+        <v>92</v>
+      </c>
     </row>
     <row r="38" spans="2:5">
       <c r="B38" s="2"/>
       <c r="C38" s="2"/>
-      <c r="D38" s="15" t="s">
-        <v>61</v>
-      </c>
-      <c r="E38" s="15" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="39" spans="2:5" ht="30">
+      <c r="D38" s="14" t="s">
+        <v>93</v>
+      </c>
+      <c r="E38" s="14" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="39" spans="2:5">
       <c r="B39" s="2"/>
       <c r="C39" s="2"/>
       <c r="D39" s="14" t="s">
-        <v>63</v>
+        <v>95</v>
       </c>
       <c r="E39" s="14" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="40" spans="2:5">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="40" spans="2:5" ht="30">
       <c r="B40" s="2"/>
       <c r="C40" s="2"/>
       <c r="D40" s="14" t="s">
-        <v>65</v>
+        <v>97</v>
       </c>
       <c r="E40" s="14" t="s">
-        <v>66</v>
+        <v>98</v>
       </c>
     </row>
     <row r="41" spans="2:5">
-      <c r="B41" s="2"/>
-      <c r="C41" s="2"/>
-      <c r="D41" s="14" t="s">
-        <v>67</v>
-      </c>
-      <c r="E41" s="14" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="42" spans="2:5">
-      <c r="B42" s="2"/>
-      <c r="C42" s="2"/>
-      <c r="D42" s="14" t="s">
-        <v>69</v>
-      </c>
-      <c r="E42" s="118" t="s">
-        <v>71</v>
-      </c>
+      <c r="B41" s="2">
+        <v>2</v>
+      </c>
+      <c r="C41" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D41" s="2"/>
+      <c r="E41" s="2"/>
+    </row>
+    <row r="42" spans="2:5" ht="18.75">
+      <c r="B42" s="2">
+        <v>3</v>
+      </c>
+      <c r="C42" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D42" s="18" t="s">
+        <v>59</v>
+      </c>
+      <c r="E42" s="2"/>
     </row>
     <row r="43" spans="2:5">
       <c r="B43" s="2"/>
       <c r="C43" s="2"/>
-      <c r="D43" s="14" t="s">
-        <v>70</v>
+      <c r="D43" s="118" t="s">
+        <v>60</v>
       </c>
       <c r="E43" s="118"/>
     </row>
     <row r="44" spans="2:5">
       <c r="B44" s="2"/>
       <c r="C44" s="2"/>
-      <c r="D44" s="14" t="s">
-        <v>72</v>
-      </c>
-      <c r="E44" s="14" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="45" spans="2:5" ht="60">
+      <c r="D44" s="15" t="s">
+        <v>61</v>
+      </c>
+      <c r="E44" s="15" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="45" spans="2:5" ht="30">
       <c r="B45" s="2"/>
       <c r="C45" s="2"/>
-      <c r="D45" s="74" t="s">
-        <v>423</v>
+      <c r="D45" s="14" t="s">
+        <v>63</v>
       </c>
       <c r="E45" s="14" t="s">
-        <v>74</v>
+        <v>64</v>
       </c>
     </row>
     <row r="46" spans="2:5">
       <c r="B46" s="2"/>
       <c r="C46" s="2"/>
       <c r="D46" s="14" t="s">
-        <v>75</v>
+        <v>65</v>
       </c>
       <c r="E46" s="14" t="s">
-        <v>76</v>
+        <v>66</v>
       </c>
     </row>
     <row r="47" spans="2:5">
       <c r="B47" s="2"/>
       <c r="C47" s="2"/>
-      <c r="D47" s="73"/>
-      <c r="E47" s="73"/>
-    </row>
-    <row r="48" spans="2:5" ht="31.5">
+      <c r="D47" s="14" t="s">
+        <v>67</v>
+      </c>
+      <c r="E47" s="14" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="48" spans="2:5">
       <c r="B48" s="2"/>
       <c r="C48" s="2"/>
-      <c r="D48" s="22" t="s">
-        <v>414</v>
-      </c>
-      <c r="E48" s="73"/>
-    </row>
-    <row r="49" spans="2:5" ht="18" customHeight="1">
+      <c r="D48" s="14" t="s">
+        <v>69</v>
+      </c>
+      <c r="E48" s="119" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="49" spans="2:5">
       <c r="B49" s="2"/>
       <c r="C49" s="2"/>
-      <c r="D49" s="69" t="s">
-        <v>416</v>
-      </c>
-      <c r="E49" s="69" t="s">
-        <v>415</v>
-      </c>
-    </row>
-    <row r="50" spans="2:5" ht="62.25" customHeight="1">
+      <c r="D49" s="14" t="s">
+        <v>70</v>
+      </c>
+      <c r="E49" s="119"/>
+    </row>
+    <row r="50" spans="2:5">
       <c r="B50" s="2"/>
       <c r="C50" s="2"/>
-      <c r="D50" s="13" t="s">
-        <v>419</v>
-      </c>
-      <c r="E50" s="77" t="s">
-        <v>417</v>
-      </c>
-    </row>
-    <row r="51" spans="2:5">
+      <c r="D50" s="14" t="s">
+        <v>72</v>
+      </c>
+      <c r="E50" s="14" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="51" spans="2:5" ht="60">
       <c r="B51" s="2"/>
       <c r="C51" s="2"/>
-      <c r="D51" s="13"/>
-      <c r="E51" s="13"/>
-    </row>
-    <row r="52" spans="2:5" ht="31.5">
+      <c r="D51" s="74" t="s">
+        <v>423</v>
+      </c>
+      <c r="E51" s="14" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="52" spans="2:5">
       <c r="B52" s="2"/>
       <c r="C52" s="2"/>
-      <c r="D52" s="22" t="s">
-        <v>418</v>
-      </c>
-      <c r="E52" s="73"/>
-    </row>
-    <row r="53" spans="2:5" ht="150">
+      <c r="D52" s="14" t="s">
+        <v>75</v>
+      </c>
+      <c r="E52" s="14" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="53" spans="2:5">
       <c r="B53" s="2"/>
       <c r="C53" s="2"/>
-      <c r="D53" s="73" t="s">
-        <v>413</v>
-      </c>
-      <c r="E53" s="2"/>
-    </row>
-    <row r="55" spans="2:5" ht="31.5">
-      <c r="B55" s="22" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="56" spans="2:5" ht="49.5" customHeight="1">
+      <c r="D53" s="73"/>
+      <c r="E53" s="73"/>
+    </row>
+    <row r="54" spans="2:5" ht="31.5">
+      <c r="B54" s="2"/>
+      <c r="C54" s="2"/>
+      <c r="D54" s="22" t="s">
+        <v>414</v>
+      </c>
+      <c r="E54" s="73"/>
+    </row>
+    <row r="55" spans="2:5" ht="18" customHeight="1">
+      <c r="B55" s="2"/>
+      <c r="C55" s="2"/>
+      <c r="D55" s="69" t="s">
+        <v>416</v>
+      </c>
+      <c r="E55" s="69" t="s">
+        <v>415</v>
+      </c>
+    </row>
+    <row r="56" spans="2:5" ht="62.25" customHeight="1">
       <c r="B56" s="2"/>
       <c r="C56" s="2"/>
-      <c r="D56" s="2" t="s">
-        <v>103</v>
-      </c>
-      <c r="E56" s="25" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="57" spans="2:5" ht="45">
+      <c r="D56" s="13" t="s">
+        <v>419</v>
+      </c>
+      <c r="E56" s="77" t="s">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="57" spans="2:5">
       <c r="B57" s="2"/>
       <c r="C57" s="2"/>
-      <c r="D57" s="2" t="s">
-        <v>105</v>
-      </c>
-      <c r="E57" s="17" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="58" spans="2:5" ht="60">
+      <c r="D57" s="13"/>
+      <c r="E57" s="13"/>
+    </row>
+    <row r="58" spans="2:5" ht="31.5">
       <c r="B58" s="2"/>
       <c r="C58" s="2"/>
-      <c r="D58" t="s">
-        <v>106</v>
-      </c>
-      <c r="E58" s="13" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="59" spans="2:5" ht="45">
+      <c r="D58" s="22" t="s">
+        <v>418</v>
+      </c>
+      <c r="E58" s="73"/>
+    </row>
+    <row r="59" spans="2:5" ht="150">
       <c r="B59" s="2"/>
       <c r="C59" s="2"/>
-      <c r="D59" s="2" t="s">
-        <v>108</v>
-      </c>
-      <c r="E59" s="17" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="60" spans="2:5" ht="45">
-      <c r="B60" s="2"/>
-      <c r="C60" s="2"/>
-      <c r="D60" s="2" t="s">
-        <v>107</v>
-      </c>
-      <c r="E60" s="17" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="61" spans="2:5" ht="30">
-      <c r="B61" s="2"/>
-      <c r="C61" s="2"/>
-      <c r="D61" s="2" t="s">
-        <v>109</v>
-      </c>
-      <c r="E61" s="17" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="62" spans="2:5" ht="30">
+      <c r="D59" s="73" t="s">
+        <v>413</v>
+      </c>
+      <c r="E59" s="2"/>
+    </row>
+    <row r="61" spans="2:5" ht="31.5">
+      <c r="B61" s="22" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="62" spans="2:5" ht="49.5" customHeight="1">
       <c r="B62" s="2"/>
       <c r="C62" s="2"/>
       <c r="D62" s="2" t="s">
-        <v>115</v>
-      </c>
-      <c r="E62" s="72" t="s">
-        <v>397</v>
-      </c>
-    </row>
-    <row r="63" spans="2:5" ht="120">
+        <v>103</v>
+      </c>
+      <c r="E62" s="25" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="63" spans="2:5" ht="45">
       <c r="B63" s="2"/>
       <c r="C63" s="2"/>
       <c r="D63" s="2" t="s">
-        <v>116</v>
+        <v>105</v>
       </c>
       <c r="E63" s="17" t="s">
-        <v>117</v>
+        <v>111</v>
       </c>
     </row>
     <row r="64" spans="2:5" ht="60">
       <c r="B64" s="2"/>
       <c r="C64" s="2"/>
-      <c r="D64" s="2" t="s">
-        <v>118</v>
-      </c>
-      <c r="E64" s="17" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="66" spans="2:5" ht="31.5">
-      <c r="B66" s="22" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="67" spans="2:5" ht="53.25" customHeight="1">
-      <c r="B67" s="32"/>
+      <c r="D64" t="s">
+        <v>106</v>
+      </c>
+      <c r="E64" s="13" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="65" spans="2:5" ht="45">
+      <c r="B65" s="2"/>
+      <c r="C65" s="2"/>
+      <c r="D65" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="E65" s="17" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="66" spans="2:5" ht="45">
+      <c r="B66" s="2"/>
+      <c r="C66" s="2"/>
+      <c r="D66" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="E66" s="17" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="67" spans="2:5" ht="30">
+      <c r="B67" s="2"/>
       <c r="C67" s="2"/>
       <c r="D67" s="2" t="s">
-        <v>436</v>
-      </c>
-      <c r="E67" s="74" t="s">
-        <v>437</v>
-      </c>
-    </row>
-    <row r="68" spans="2:5" ht="53.25" customHeight="1">
-      <c r="B68" s="32"/>
+        <v>109</v>
+      </c>
+      <c r="E67" s="17" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="68" spans="2:5" ht="30">
+      <c r="B68" s="2"/>
       <c r="C68" s="2"/>
       <c r="D68" s="2" t="s">
-        <v>438</v>
-      </c>
-      <c r="E68" s="74" t="s">
-        <v>439</v>
-      </c>
-    </row>
-    <row r="69" spans="2:5" ht="53.25" customHeight="1">
-      <c r="B69" s="32"/>
+        <v>115</v>
+      </c>
+      <c r="E68" s="72" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="69" spans="2:5" ht="120">
+      <c r="B69" s="2"/>
       <c r="C69" s="2"/>
       <c r="D69" s="2" t="s">
-        <v>440</v>
-      </c>
-      <c r="E69" s="74" t="s">
-        <v>441</v>
-      </c>
-    </row>
-    <row r="70" spans="2:5" ht="205.5" customHeight="1">
-      <c r="B70" s="32"/>
+        <v>116</v>
+      </c>
+      <c r="E69" s="17" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="70" spans="2:5" ht="60">
+      <c r="B70" s="2"/>
       <c r="C70" s="2"/>
-      <c r="D70" s="78" t="s">
-        <v>442</v>
-      </c>
-      <c r="E70" s="13" t="s">
-        <v>443</v>
-      </c>
-    </row>
-    <row r="71" spans="2:5" ht="35.25" customHeight="1">
-      <c r="B71" s="32"/>
-      <c r="C71" s="22" t="s">
-        <v>445</v>
-      </c>
-      <c r="D71" s="78"/>
-      <c r="E71" s="13"/>
-    </row>
-    <row r="72" spans="2:5" ht="52.5" customHeight="1">
-      <c r="B72" s="32"/>
-      <c r="C72" s="2"/>
-      <c r="D72" s="78" t="s">
-        <v>446</v>
-      </c>
-      <c r="E72" s="13" t="s">
-        <v>444</v>
-      </c>
-    </row>
-    <row r="73" spans="2:5" ht="52.5" customHeight="1">
+      <c r="D70" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="E70" s="17" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="72" spans="2:5" ht="31.5">
+      <c r="B72" s="22" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="73" spans="2:5" ht="53.25" customHeight="1">
       <c r="B73" s="32"/>
       <c r="C73" s="2"/>
-      <c r="D73" s="78" t="s">
-        <v>447</v>
-      </c>
-      <c r="E73" s="13" t="s">
-        <v>453</v>
-      </c>
-    </row>
-    <row r="74" spans="2:5" ht="36" customHeight="1">
+      <c r="D73" s="2" t="s">
+        <v>436</v>
+      </c>
+      <c r="E73" s="74" t="s">
+        <v>437</v>
+      </c>
+    </row>
+    <row r="74" spans="2:5" ht="53.25" customHeight="1">
       <c r="B74" s="32"/>
       <c r="C74" s="2"/>
-      <c r="D74" s="78" t="s">
-        <v>449</v>
-      </c>
-      <c r="E74" s="13" t="s">
-        <v>448</v>
-      </c>
-    </row>
-    <row r="75" spans="2:5" ht="120.75" customHeight="1">
+      <c r="D74" s="2" t="s">
+        <v>438</v>
+      </c>
+      <c r="E74" s="74" t="s">
+        <v>439</v>
+      </c>
+    </row>
+    <row r="75" spans="2:5" ht="53.25" customHeight="1">
       <c r="B75" s="32"/>
       <c r="C75" s="2"/>
-      <c r="D75" s="78" t="s">
-        <v>450</v>
-      </c>
-      <c r="E75" s="13" t="s">
-        <v>454</v>
-      </c>
-    </row>
-    <row r="76" spans="2:5" ht="31.5">
+      <c r="D75" s="2" t="s">
+        <v>440</v>
+      </c>
+      <c r="E75" s="74" t="s">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="76" spans="2:5" ht="205.5" customHeight="1">
       <c r="B76" s="32"/>
       <c r="C76" s="2"/>
-      <c r="D76" s="80" t="s">
+      <c r="D76" s="78" t="s">
+        <v>442</v>
+      </c>
+      <c r="E76" s="13" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="77" spans="2:5" ht="35.25" customHeight="1">
+      <c r="B77" s="32"/>
+      <c r="C77" s="22" t="s">
+        <v>445</v>
+      </c>
+      <c r="D77" s="78"/>
+      <c r="E77" s="13"/>
+    </row>
+    <row r="78" spans="2:5" ht="52.5" customHeight="1">
+      <c r="B78" s="32"/>
+      <c r="C78" s="2"/>
+      <c r="D78" s="78" t="s">
+        <v>446</v>
+      </c>
+      <c r="E78" s="13" t="s">
+        <v>444</v>
+      </c>
+    </row>
+    <row r="79" spans="2:5" ht="52.5" customHeight="1">
+      <c r="B79" s="32"/>
+      <c r="C79" s="2"/>
+      <c r="D79" s="78" t="s">
+        <v>447</v>
+      </c>
+      <c r="E79" s="13" t="s">
+        <v>453</v>
+      </c>
+    </row>
+    <row r="80" spans="2:5" ht="36" customHeight="1">
+      <c r="B80" s="32"/>
+      <c r="C80" s="2"/>
+      <c r="D80" s="78" t="s">
+        <v>449</v>
+      </c>
+      <c r="E80" s="13" t="s">
+        <v>448</v>
+      </c>
+    </row>
+    <row r="81" spans="2:5" ht="120.75" customHeight="1">
+      <c r="B81" s="32"/>
+      <c r="C81" s="2"/>
+      <c r="D81" s="78" t="s">
+        <v>450</v>
+      </c>
+      <c r="E81" s="13" t="s">
+        <v>454</v>
+      </c>
+    </row>
+    <row r="82" spans="2:5" ht="31.5">
+      <c r="B82" s="32"/>
+      <c r="C82" s="2"/>
+      <c r="D82" s="80" t="s">
         <v>451</v>
       </c>
-      <c r="E76" s="13"/>
-    </row>
-    <row r="77" spans="2:5" ht="66" customHeight="1">
-      <c r="B77" s="32"/>
-      <c r="C77" s="2"/>
-      <c r="D77" s="79" t="s">
+      <c r="E82" s="13"/>
+    </row>
+    <row r="83" spans="2:5" ht="66" customHeight="1">
+      <c r="B83" s="32"/>
+      <c r="C83" s="2"/>
+      <c r="D83" s="79" t="s">
         <v>452</v>
       </c>
-      <c r="E77" s="13"/>
-    </row>
-    <row r="78" spans="2:5" ht="225">
-      <c r="B78" s="2"/>
-      <c r="C78" s="2"/>
-      <c r="D78" s="2" t="s">
-        <v>120</v>
-      </c>
-      <c r="E78" s="21" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="79" spans="2:5">
-      <c r="B79" s="2"/>
-      <c r="C79" s="2"/>
-      <c r="D79" s="2"/>
-      <c r="E79" s="74"/>
-    </row>
-    <row r="80" spans="2:5" ht="30">
-      <c r="B80" s="2"/>
-      <c r="C80" s="2"/>
-      <c r="D80" s="2" t="s">
-        <v>122</v>
-      </c>
-      <c r="E80" s="17" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="81" spans="2:5" ht="90">
-      <c r="B81" s="2"/>
-      <c r="C81" s="2"/>
-      <c r="D81" s="2" t="s">
-        <v>121</v>
-      </c>
-      <c r="E81" s="17" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="82" spans="2:5" ht="45">
-      <c r="B82" s="2"/>
-      <c r="C82" s="2"/>
-      <c r="D82" s="2" t="s">
-        <v>126</v>
-      </c>
-      <c r="E82" s="21" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="83" spans="2:5" ht="60">
-      <c r="B83" s="2"/>
-      <c r="C83" s="2"/>
-      <c r="D83" s="2" t="s">
-        <v>127</v>
-      </c>
-      <c r="E83" s="21" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="84" spans="2:5" ht="90">
+      <c r="E83" s="13"/>
+    </row>
+    <row r="84" spans="2:5" ht="225">
       <c r="B84" s="2"/>
       <c r="C84" s="2"/>
       <c r="D84" s="2" t="s">
-        <v>130</v>
+        <v>120</v>
       </c>
       <c r="E84" s="21" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="85" spans="2:5" ht="30">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="85" spans="2:5">
       <c r="B85" s="2"/>
       <c r="C85" s="2"/>
-      <c r="D85" s="2" t="s">
-        <v>132</v>
-      </c>
-      <c r="E85" s="21" t="s">
-        <v>133</v>
-      </c>
+      <c r="D85" s="2"/>
+      <c r="E85" s="74"/>
     </row>
     <row r="86" spans="2:5" ht="30">
       <c r="B86" s="2"/>
       <c r="C86" s="2"/>
       <c r="D86" s="2" t="s">
-        <v>134</v>
-      </c>
-      <c r="E86" s="21" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="87" spans="2:5" ht="60">
+        <v>122</v>
+      </c>
+      <c r="E86" s="17" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="87" spans="2:5" ht="90">
       <c r="B87" s="2"/>
       <c r="C87" s="2"/>
       <c r="D87" s="2" t="s">
-        <v>137</v>
-      </c>
-      <c r="E87" s="21" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="88" spans="2:5" ht="90">
+        <v>121</v>
+      </c>
+      <c r="E87" s="17" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="88" spans="2:5" ht="45">
       <c r="B88" s="2"/>
       <c r="C88" s="2"/>
       <c r="D88" s="2" t="s">
-        <v>138</v>
+        <v>126</v>
       </c>
       <c r="E88" s="21" t="s">
-        <v>139</v>
+        <v>129</v>
       </c>
     </row>
     <row r="89" spans="2:5" ht="60">
       <c r="B89" s="2"/>
       <c r="C89" s="2"/>
       <c r="D89" s="2" t="s">
-        <v>140</v>
+        <v>127</v>
       </c>
       <c r="E89" s="21" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="90" spans="2:5">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="90" spans="2:5" ht="90">
       <c r="B90" s="2"/>
       <c r="C90" s="2"/>
-      <c r="D90" s="2"/>
-      <c r="E90" s="21"/>
-    </row>
-    <row r="91" spans="2:5">
+      <c r="D90" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="E90" s="21" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="91" spans="2:5" ht="30">
       <c r="B91" s="2"/>
       <c r="C91" s="2"/>
-      <c r="D91" s="2"/>
-      <c r="E91" s="21"/>
-    </row>
-    <row r="92" spans="2:5">
+      <c r="D91" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="E91" s="21" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="92" spans="2:5" ht="30">
       <c r="B92" s="2"/>
       <c r="C92" s="2"/>
-      <c r="D92" s="2"/>
-      <c r="E92" s="21"/>
-    </row>
-    <row r="93" spans="2:5">
+      <c r="D92" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="E92" s="21" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="93" spans="2:5" ht="60">
       <c r="B93" s="2"/>
       <c r="C93" s="2"/>
-      <c r="D93" s="2"/>
-      <c r="E93" s="21"/>
-    </row>
-    <row r="94" spans="2:5">
+      <c r="D93" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="E93" s="21" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="94" spans="2:5" ht="90">
       <c r="B94" s="2"/>
       <c r="C94" s="2"/>
-      <c r="D94" s="2"/>
-      <c r="E94" s="21"/>
-    </row>
-    <row r="95" spans="2:5">
+      <c r="D94" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="E94" s="21" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="95" spans="2:5" ht="60">
       <c r="B95" s="2"/>
       <c r="C95" s="2"/>
-      <c r="D95" s="2"/>
-      <c r="E95" s="21"/>
+      <c r="D95" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="E95" s="21" t="s">
+        <v>142</v>
+      </c>
     </row>
     <row r="96" spans="2:5">
       <c r="B96" s="2"/>
       <c r="C96" s="2"/>
       <c r="D96" s="2"/>
-      <c r="E96" s="26"/>
+      <c r="E96" s="21"/>
     </row>
     <row r="97" spans="2:5">
       <c r="B97" s="2"/>
       <c r="C97" s="2"/>
       <c r="D97" s="2"/>
-      <c r="E97" s="2"/>
+      <c r="E97" s="21"/>
     </row>
     <row r="98" spans="2:5">
       <c r="B98" s="2"/>
       <c r="C98" s="2"/>
       <c r="D98" s="2"/>
-      <c r="E98" s="2"/>
+      <c r="E98" s="21"/>
     </row>
     <row r="99" spans="2:5">
       <c r="B99" s="2"/>
       <c r="C99" s="2"/>
       <c r="D99" s="2"/>
-      <c r="E99" s="2"/>
+      <c r="E99" s="21"/>
     </row>
     <row r="100" spans="2:5">
       <c r="B100" s="2"/>
       <c r="C100" s="2"/>
       <c r="D100" s="2"/>
-      <c r="E100" s="2"/>
-    </row>
-    <row r="101" spans="2:5" ht="60">
+      <c r="E100" s="21"/>
+    </row>
+    <row r="101" spans="2:5">
       <c r="B101" s="2"/>
       <c r="C101" s="2"/>
-      <c r="D101" s="2" t="s">
-        <v>150</v>
-      </c>
-      <c r="E101" s="26" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="102" spans="2:5" ht="75">
+      <c r="D101" s="2"/>
+      <c r="E101" s="21"/>
+    </row>
+    <row r="102" spans="2:5">
       <c r="B102" s="2"/>
       <c r="C102" s="2"/>
-      <c r="D102" s="2" t="s">
-        <v>152</v>
-      </c>
-      <c r="E102" s="26" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="103" spans="2:5" ht="60">
+      <c r="D102" s="2"/>
+      <c r="E102" s="26"/>
+    </row>
+    <row r="103" spans="2:5">
       <c r="B103" s="2"/>
       <c r="C103" s="2"/>
-      <c r="D103" s="2" t="s">
-        <v>156</v>
-      </c>
-      <c r="E103" s="26" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="104" spans="2:5" ht="32.25" customHeight="1">
+      <c r="D103" s="2"/>
+      <c r="E103" s="2"/>
+    </row>
+    <row r="104" spans="2:5">
       <c r="B104" s="2"/>
       <c r="C104" s="2"/>
-      <c r="D104" s="2" t="s">
-        <v>158</v>
-      </c>
-      <c r="E104" s="26" t="s">
-        <v>159</v>
-      </c>
+      <c r="D104" s="2"/>
+      <c r="E104" s="2"/>
     </row>
     <row r="105" spans="2:5">
       <c r="B105" s="2"/>
       <c r="C105" s="2"/>
-      <c r="D105" s="2" t="s">
-        <v>160</v>
-      </c>
-      <c r="E105" s="26" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="106" spans="2:5" ht="75">
+      <c r="D105" s="2"/>
+      <c r="E105" s="2"/>
+    </row>
+    <row r="106" spans="2:5">
       <c r="B106" s="2"/>
       <c r="C106" s="2"/>
-      <c r="D106" s="2" t="s">
-        <v>162</v>
-      </c>
-      <c r="E106" s="26" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="107" spans="2:5" ht="45">
+      <c r="D106" s="2"/>
+      <c r="E106" s="2"/>
+    </row>
+    <row r="107" spans="2:5" ht="60">
       <c r="B107" s="2"/>
-      <c r="C107" s="32" t="s">
-        <v>425</v>
-      </c>
-      <c r="D107" s="2"/>
-      <c r="E107" s="40" t="s">
-        <v>426</v>
-      </c>
-    </row>
-    <row r="108" spans="2:5" ht="31.5">
+      <c r="C107" s="2"/>
+      <c r="D107" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="E107" s="26" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="108" spans="2:5" ht="75">
       <c r="B108" s="2"/>
-      <c r="C108" s="22"/>
-      <c r="D108" s="2"/>
-      <c r="E108" s="74"/>
-    </row>
-    <row r="109" spans="2:5" ht="135">
+      <c r="C108" s="2"/>
+      <c r="D108" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="E108" s="26" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="109" spans="2:5" ht="60">
       <c r="B109" s="2"/>
       <c r="C109" s="2"/>
       <c r="D109" s="2" t="s">
-        <v>164</v>
+        <v>156</v>
       </c>
       <c r="E109" s="26" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="110" spans="2:5" ht="90">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="110" spans="2:5" ht="32.25" customHeight="1">
       <c r="B110" s="2"/>
       <c r="C110" s="2"/>
       <c r="D110" s="2" t="s">
-        <v>166</v>
+        <v>158</v>
       </c>
       <c r="E110" s="26" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="111" spans="2:5" ht="45">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="111" spans="2:5">
       <c r="B111" s="2"/>
       <c r="C111" s="2"/>
       <c r="D111" s="2" t="s">
-        <v>168</v>
+        <v>160</v>
       </c>
       <c r="E111" s="26" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="112" spans="2:5">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="112" spans="2:5" ht="75">
       <c r="B112" s="2"/>
       <c r="C112" s="2"/>
       <c r="D112" s="2" t="s">
-        <v>170</v>
+        <v>162</v>
       </c>
       <c r="E112" s="26" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="113" spans="2:5" ht="30">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="113" spans="2:5" ht="45">
       <c r="B113" s="2"/>
-      <c r="C113" s="2"/>
-      <c r="D113" s="26" t="s">
-        <v>172</v>
-      </c>
-      <c r="E113" s="26" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="114" spans="2:5">
+      <c r="C113" s="32" t="s">
+        <v>425</v>
+      </c>
+      <c r="D113" s="2"/>
+      <c r="E113" s="40" t="s">
+        <v>426</v>
+      </c>
+    </row>
+    <row r="114" spans="2:5" ht="31.5">
       <c r="B114" s="2"/>
-      <c r="C114" s="2"/>
-      <c r="D114" s="2" t="s">
-        <v>174</v>
-      </c>
-      <c r="E114" s="26"/>
-    </row>
-    <row r="115" spans="2:5">
+      <c r="C114" s="22"/>
+      <c r="D114" s="2"/>
+      <c r="E114" s="74"/>
+    </row>
+    <row r="115" spans="2:5" ht="135">
       <c r="B115" s="2"/>
       <c r="C115" s="2"/>
-      <c r="D115" s="15" t="s">
-        <v>175</v>
-      </c>
-      <c r="E115" s="15" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="116" spans="2:5">
+      <c r="D115" s="2" t="s">
+        <v>164</v>
+      </c>
+      <c r="E115" s="26" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="116" spans="2:5" ht="90">
       <c r="B116" s="2"/>
       <c r="C116" s="2"/>
-      <c r="D116" s="26" t="s">
-        <v>177</v>
+      <c r="D116" s="2" t="s">
+        <v>166</v>
       </c>
       <c r="E116" s="26" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="117" spans="2:5">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="117" spans="2:5" ht="45">
       <c r="B117" s="2"/>
       <c r="C117" s="2"/>
-      <c r="D117" s="26" t="s">
-        <v>179</v>
+      <c r="D117" s="2" t="s">
+        <v>168</v>
       </c>
       <c r="E117" s="26" t="s">
-        <v>180</v>
+        <v>169</v>
       </c>
     </row>
     <row r="118" spans="2:5">
       <c r="B118" s="2"/>
       <c r="C118" s="2"/>
-      <c r="D118" s="26" t="s">
-        <v>181</v>
+      <c r="D118" s="2" t="s">
+        <v>170</v>
       </c>
       <c r="E118" s="26" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="119" spans="2:5">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="119" spans="2:5" ht="30">
       <c r="B119" s="2"/>
       <c r="C119" s="2"/>
       <c r="D119" s="26" t="s">
-        <v>183</v>
+        <v>172</v>
       </c>
       <c r="E119" s="26" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="120" spans="2:5" ht="31.5">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="120" spans="2:5">
       <c r="B120" s="2"/>
-      <c r="C120" s="22" t="s">
-        <v>185</v>
-      </c>
-      <c r="D120" s="2"/>
+      <c r="C120" s="2"/>
+      <c r="D120" s="2" t="s">
+        <v>174</v>
+      </c>
       <c r="E120" s="26"/>
     </row>
-    <row r="121" spans="2:5" ht="105">
+    <row r="121" spans="2:5">
       <c r="B121" s="2"/>
       <c r="C121" s="2"/>
-      <c r="D121" s="2" t="s">
-        <v>186</v>
-      </c>
-      <c r="E121" s="74" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="122" spans="2:5" ht="120">
+      <c r="D121" s="15" t="s">
+        <v>175</v>
+      </c>
+      <c r="E121" s="15" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="122" spans="2:5">
       <c r="B122" s="2"/>
       <c r="C122" s="2"/>
-      <c r="D122" s="2" t="s">
-        <v>187</v>
-      </c>
-      <c r="E122" s="74" t="s">
-        <v>424</v>
-      </c>
-    </row>
-    <row r="123" spans="2:5" ht="255">
+      <c r="D122" s="26" t="s">
+        <v>177</v>
+      </c>
+      <c r="E122" s="26" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="123" spans="2:5">
       <c r="B123" s="2"/>
       <c r="C123" s="2"/>
-      <c r="D123" s="2" t="s">
-        <v>188</v>
+      <c r="D123" s="26" t="s">
+        <v>179</v>
       </c>
       <c r="E123" s="26" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="124" spans="2:5" ht="180">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="124" spans="2:5">
       <c r="B124" s="2"/>
       <c r="C124" s="2"/>
-      <c r="D124" s="2" t="s">
-        <v>190</v>
-      </c>
-      <c r="E124" s="28" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="125" spans="2:5" ht="30">
+      <c r="D124" s="26" t="s">
+        <v>181</v>
+      </c>
+      <c r="E124" s="26" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="125" spans="2:5">
       <c r="B125" s="2"/>
       <c r="C125" s="2"/>
-      <c r="D125" s="28" t="s">
-        <v>195</v>
-      </c>
-      <c r="E125" s="28"/>
-    </row>
-    <row r="126" spans="2:5" ht="30">
+      <c r="D125" s="26" t="s">
+        <v>183</v>
+      </c>
+      <c r="E125" s="26" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="126" spans="2:5" ht="31.5">
       <c r="B126" s="2"/>
-      <c r="C126" s="2"/>
-      <c r="D126" s="28" t="s">
-        <v>196</v>
-      </c>
-      <c r="E126" s="28"/>
-    </row>
-    <row r="127" spans="2:5" ht="30">
+      <c r="C126" s="22" t="s">
+        <v>185</v>
+      </c>
+      <c r="D126" s="2"/>
+      <c r="E126" s="26"/>
+    </row>
+    <row r="127" spans="2:5" ht="105">
       <c r="B127" s="2"/>
       <c r="C127" s="2"/>
-      <c r="D127" s="28" t="s">
-        <v>198</v>
-      </c>
-      <c r="E127" s="28"/>
-    </row>
-    <row r="128" spans="2:5" ht="45">
+      <c r="D127" s="2" t="s">
+        <v>186</v>
+      </c>
+      <c r="E127" s="74" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="128" spans="2:5" ht="120">
       <c r="B128" s="2"/>
       <c r="C128" s="2"/>
-      <c r="D128" s="28" t="s">
-        <v>192</v>
-      </c>
-      <c r="E128" s="28"/>
-    </row>
-    <row r="129" spans="2:5">
+      <c r="D128" s="2" t="s">
+        <v>187</v>
+      </c>
+      <c r="E128" s="74" t="s">
+        <v>424</v>
+      </c>
+    </row>
+    <row r="129" spans="2:5" ht="255">
       <c r="B129" s="2"/>
       <c r="C129" s="2"/>
-      <c r="D129" s="28" t="s">
-        <v>199</v>
-      </c>
-      <c r="E129" s="28"/>
-    </row>
-    <row r="130" spans="2:5" ht="60">
+      <c r="D129" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="E129" s="26" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="130" spans="2:5" ht="180">
       <c r="B130" s="2"/>
       <c r="C130" s="2"/>
-      <c r="D130" s="28" t="s">
-        <v>200</v>
-      </c>
-      <c r="E130" s="28"/>
+      <c r="D130" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="E130" s="28" t="s">
+        <v>191</v>
+      </c>
     </row>
     <row r="131" spans="2:5" ht="30">
       <c r="B131" s="2"/>
       <c r="C131" s="2"/>
       <c r="D131" s="28" t="s">
-        <v>201</v>
+        <v>195</v>
       </c>
       <c r="E131" s="28"/>
     </row>
-    <row r="132" spans="2:5">
+    <row r="132" spans="2:5" ht="30">
       <c r="B132" s="2"/>
       <c r="C132" s="2"/>
       <c r="D132" s="28" t="s">
-        <v>202</v>
+        <v>196</v>
       </c>
       <c r="E132" s="28"/>
     </row>
@@ -16328,104 +17598,116 @@
       <c r="B133" s="2"/>
       <c r="C133" s="2"/>
       <c r="D133" s="28" t="s">
-        <v>193</v>
+        <v>198</v>
       </c>
       <c r="E133" s="28"/>
     </row>
-    <row r="134" spans="2:5" ht="30">
+    <row r="134" spans="2:5" ht="45">
       <c r="B134" s="2"/>
       <c r="C134" s="2"/>
       <c r="D134" s="28" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="E134" s="28"/>
     </row>
     <row r="135" spans="2:5">
       <c r="B135" s="2"/>
       <c r="C135" s="2"/>
-      <c r="D135" s="28"/>
-      <c r="E135" s="26"/>
-    </row>
-    <row r="137" spans="2:5" ht="31.5">
-      <c r="C137" s="22" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="138" spans="2:5" ht="90">
+      <c r="D135" s="28" t="s">
+        <v>199</v>
+      </c>
+      <c r="E135" s="28"/>
+    </row>
+    <row r="136" spans="2:5" ht="60">
+      <c r="B136" s="2"/>
+      <c r="C136" s="2"/>
+      <c r="D136" s="28" t="s">
+        <v>200</v>
+      </c>
+      <c r="E136" s="28"/>
+    </row>
+    <row r="137" spans="2:5" ht="30">
+      <c r="B137" s="2"/>
+      <c r="C137" s="2"/>
+      <c r="D137" s="28" t="s">
+        <v>201</v>
+      </c>
+      <c r="E137" s="28"/>
+    </row>
+    <row r="138" spans="2:5">
       <c r="B138" s="2"/>
       <c r="C138" s="2"/>
-      <c r="D138" s="2" t="s">
-        <v>144</v>
-      </c>
-      <c r="E138" s="21" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="139" spans="2:5" ht="90">
+      <c r="D138" s="28" t="s">
+        <v>202</v>
+      </c>
+      <c r="E138" s="28"/>
+    </row>
+    <row r="139" spans="2:5" ht="30">
       <c r="B139" s="2"/>
       <c r="C139" s="2"/>
       <c r="D139" s="28" t="s">
-        <v>146</v>
-      </c>
-      <c r="E139" s="21" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="140" spans="2:5" ht="105">
+        <v>193</v>
+      </c>
+      <c r="E139" s="28"/>
+    </row>
+    <row r="140" spans="2:5" ht="30">
       <c r="B140" s="2"/>
       <c r="C140" s="2"/>
-      <c r="D140" s="2" t="s">
-        <v>155</v>
-      </c>
-      <c r="E140" s="21" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="141" spans="2:5" ht="90">
+      <c r="D140" s="28" t="s">
+        <v>194</v>
+      </c>
+      <c r="E140" s="28"/>
+    </row>
+    <row r="141" spans="2:5">
       <c r="B141" s="2"/>
       <c r="C141" s="2"/>
-      <c r="D141" s="2" t="s">
-        <v>154</v>
-      </c>
-      <c r="E141" s="21" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="142" spans="2:5">
-      <c r="B142" s="2"/>
-      <c r="C142" s="2"/>
-      <c r="D142" s="2"/>
-      <c r="E142" s="21"/>
-    </row>
-    <row r="143" spans="2:5">
-      <c r="B143" s="2"/>
-      <c r="C143" s="2"/>
-      <c r="D143" s="2"/>
-      <c r="E143" s="21"/>
-    </row>
-    <row r="144" spans="2:5">
+      <c r="D141" s="28"/>
+      <c r="E141" s="26"/>
+    </row>
+    <row r="143" spans="2:5" ht="31.5">
+      <c r="C143" s="22" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="144" spans="2:5" ht="90">
       <c r="B144" s="2"/>
       <c r="C144" s="2"/>
-      <c r="D144" s="2"/>
-      <c r="E144" s="21"/>
-    </row>
-    <row r="145" spans="2:5">
+      <c r="D144" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="E144" s="21" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="145" spans="2:5" ht="90">
       <c r="B145" s="2"/>
       <c r="C145" s="2"/>
-      <c r="D145" s="2"/>
-      <c r="E145" s="21"/>
-    </row>
-    <row r="146" spans="2:5">
+      <c r="D145" s="28" t="s">
+        <v>146</v>
+      </c>
+      <c r="E145" s="21" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="146" spans="2:5" ht="105">
       <c r="B146" s="2"/>
       <c r="C146" s="2"/>
-      <c r="D146" s="2"/>
-      <c r="E146" s="21"/>
-    </row>
-    <row r="147" spans="2:5">
+      <c r="D146" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="E146" s="21" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="147" spans="2:5" ht="90">
       <c r="B147" s="2"/>
       <c r="C147" s="2"/>
-      <c r="D147" s="2"/>
-      <c r="E147" s="21"/>
+      <c r="D147" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="E147" s="21" t="s">
+        <v>149</v>
+      </c>
     </row>
     <row r="148" spans="2:5">
       <c r="B148" s="2"/>
@@ -16440,141 +17722,177 @@
       <c r="E149" s="21"/>
     </row>
     <row r="150" spans="2:5">
-      <c r="E150" s="27"/>
-    </row>
-    <row r="185" spans="2:5" ht="31.5">
-      <c r="B185" s="22" t="s">
+      <c r="B150" s="2"/>
+      <c r="C150" s="2"/>
+      <c r="D150" s="2"/>
+      <c r="E150" s="21"/>
+    </row>
+    <row r="151" spans="2:5">
+      <c r="B151" s="2"/>
+      <c r="C151" s="2"/>
+      <c r="D151" s="2"/>
+      <c r="E151" s="21"/>
+    </row>
+    <row r="152" spans="2:5">
+      <c r="B152" s="2"/>
+      <c r="C152" s="2"/>
+      <c r="D152" s="2"/>
+      <c r="E152" s="21"/>
+    </row>
+    <row r="153" spans="2:5">
+      <c r="B153" s="2"/>
+      <c r="C153" s="2"/>
+      <c r="D153" s="2"/>
+      <c r="E153" s="21"/>
+    </row>
+    <row r="154" spans="2:5">
+      <c r="B154" s="2"/>
+      <c r="C154" s="2"/>
+      <c r="D154" s="2"/>
+      <c r="E154" s="21"/>
+    </row>
+    <row r="155" spans="2:5">
+      <c r="B155" s="2"/>
+      <c r="C155" s="2"/>
+      <c r="D155" s="2"/>
+      <c r="E155" s="21"/>
+    </row>
+    <row r="156" spans="2:5">
+      <c r="E156" s="27"/>
+    </row>
+    <row r="191" spans="2:5" ht="31.5">
+      <c r="B191" s="22" t="s">
         <v>203</v>
       </c>
-      <c r="C185" s="23"/>
-      <c r="D185" s="23"/>
-      <c r="E185" s="24"/>
-    </row>
-    <row r="186" spans="2:5">
-      <c r="B186" s="19" t="s">
+      <c r="C191" s="23"/>
+      <c r="D191" s="23"/>
+      <c r="E191" s="24"/>
+    </row>
+    <row r="192" spans="2:5">
+      <c r="B192" s="19" t="s">
         <v>3</v>
       </c>
-      <c r="C186" s="19"/>
-      <c r="D186" s="19" t="s">
+      <c r="C192" s="19"/>
+      <c r="D192" s="19" t="s">
         <v>35</v>
       </c>
-      <c r="E186" s="19" t="s">
+      <c r="E192" s="19" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="187" spans="2:5" ht="165">
-      <c r="B187" s="2"/>
-      <c r="C187" s="2"/>
-      <c r="D187" s="10" t="s">
-        <v>204</v>
-      </c>
-      <c r="E187" s="29" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="188" spans="2:5">
-      <c r="B188" s="2"/>
-      <c r="C188" s="2"/>
-      <c r="D188" s="31" t="s">
-        <v>206</v>
-      </c>
-      <c r="E188" s="31" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="189" spans="2:5">
-      <c r="B189" s="2"/>
-      <c r="C189" s="2"/>
-      <c r="D189" s="2" t="s">
-        <v>208</v>
-      </c>
-      <c r="E189" s="29" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="190" spans="2:5" ht="30">
-      <c r="B190" s="2"/>
-      <c r="C190" s="2"/>
-      <c r="D190" s="2" t="s">
-        <v>210</v>
-      </c>
-      <c r="E190" s="29" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="191" spans="2:5">
-      <c r="B191" s="2"/>
-      <c r="C191" s="2"/>
-      <c r="D191" s="2" t="s">
-        <v>212</v>
-      </c>
-      <c r="E191" s="29" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="192" spans="2:5">
-      <c r="B192" s="2"/>
-      <c r="C192" s="2"/>
-      <c r="D192" s="2" t="s">
-        <v>214</v>
-      </c>
-      <c r="E192" s="29" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="193" spans="2:5">
+    <row r="193" spans="2:5" ht="165">
       <c r="B193" s="2"/>
       <c r="C193" s="2"/>
-      <c r="D193" s="2" t="s">
-        <v>216</v>
+      <c r="D193" s="10" t="s">
+        <v>204</v>
       </c>
       <c r="E193" s="29" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="194" spans="2:5" ht="74.25" customHeight="1">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="194" spans="2:5">
       <c r="B194" s="2"/>
-      <c r="C194" s="32"/>
-      <c r="D194" s="33" t="s">
-        <v>218</v>
-      </c>
-      <c r="E194" s="30" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="195" spans="2:5" ht="78.75">
+      <c r="C194" s="2"/>
+      <c r="D194" s="31" t="s">
+        <v>206</v>
+      </c>
+      <c r="E194" s="31" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="195" spans="2:5">
       <c r="B195" s="2"/>
-      <c r="C195" s="32"/>
-      <c r="D195" s="33" t="s">
-        <v>212</v>
-      </c>
-      <c r="E195" s="30" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="196" spans="2:5" ht="93.75">
+      <c r="C195" s="2"/>
+      <c r="D195" s="2" t="s">
+        <v>208</v>
+      </c>
+      <c r="E195" s="29" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="196" spans="2:5" ht="30">
       <c r="B196" s="2"/>
-      <c r="C196" s="32"/>
-      <c r="D196" s="1" t="s">
-        <v>221</v>
-      </c>
-      <c r="E196" s="30" t="s">
-        <v>222</v>
+      <c r="C196" s="2"/>
+      <c r="D196" s="2" t="s">
+        <v>210</v>
+      </c>
+      <c r="E196" s="29" t="s">
+        <v>211</v>
       </c>
     </row>
     <row r="197" spans="2:5">
       <c r="B197" s="2"/>
       <c r="C197" s="2"/>
-      <c r="D197" s="2"/>
-      <c r="E197" s="29"/>
+      <c r="D197" s="2" t="s">
+        <v>212</v>
+      </c>
+      <c r="E197" s="29" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="198" spans="2:5">
+      <c r="B198" s="2"/>
+      <c r="C198" s="2"/>
+      <c r="D198" s="2" t="s">
+        <v>214</v>
+      </c>
+      <c r="E198" s="29" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="199" spans="2:5">
+      <c r="B199" s="2"/>
+      <c r="C199" s="2"/>
+      <c r="D199" s="2" t="s">
+        <v>216</v>
+      </c>
+      <c r="E199" s="29" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="200" spans="2:5" ht="74.25" customHeight="1">
+      <c r="B200" s="2"/>
+      <c r="C200" s="32"/>
+      <c r="D200" s="33" t="s">
+        <v>218</v>
+      </c>
+      <c r="E200" s="30" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="201" spans="2:5" ht="78.75">
+      <c r="B201" s="2"/>
+      <c r="C201" s="32"/>
+      <c r="D201" s="33" t="s">
+        <v>212</v>
+      </c>
+      <c r="E201" s="30" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="202" spans="2:5" ht="93.75">
+      <c r="B202" s="2"/>
+      <c r="C202" s="32"/>
+      <c r="D202" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="E202" s="30" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="203" spans="2:5">
+      <c r="B203" s="2"/>
+      <c r="C203" s="2"/>
+      <c r="D203" s="2"/>
+      <c r="E203" s="29"/>
     </row>
   </sheetData>
   <mergeCells count="5">
-    <mergeCell ref="D14:E14"/>
-    <mergeCell ref="D37:E37"/>
-    <mergeCell ref="E42:E43"/>
-    <mergeCell ref="D21:E21"/>
-    <mergeCell ref="D28:E28"/>
+    <mergeCell ref="D20:E20"/>
+    <mergeCell ref="D43:E43"/>
+    <mergeCell ref="E48:E49"/>
+    <mergeCell ref="D27:E27"/>
+    <mergeCell ref="D34:E34"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -16586,7 +17904,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B3:C13"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
@@ -16964,27 +18282,27 @@
       </c>
     </row>
     <row r="49" spans="1:3">
-      <c r="A49" s="118" t="s">
+      <c r="A49" s="119" t="s">
         <v>338</v>
       </c>
       <c r="B49" s="53" t="s">
         <v>339</v>
       </c>
-      <c r="C49" s="118" t="s">
+      <c r="C49" s="119" t="s">
         <v>341</v>
       </c>
     </row>
     <row r="50" spans="1:3">
-      <c r="A50" s="118"/>
+      <c r="A50" s="119"/>
       <c r="B50" s="53"/>
-      <c r="C50" s="118"/>
+      <c r="C50" s="119"/>
     </row>
     <row r="51" spans="1:3">
-      <c r="A51" s="118"/>
+      <c r="A51" s="119"/>
       <c r="B51" s="53" t="s">
         <v>340</v>
       </c>
-      <c r="C51" s="118"/>
+      <c r="C51" s="119"/>
     </row>
     <row r="52" spans="1:3">
       <c r="A52" s="53" t="s">
@@ -17014,22 +18332,22 @@
       <c r="B56" s="58"/>
     </row>
     <row r="57" spans="1:3" ht="32.25" customHeight="1">
-      <c r="B57" s="122" t="s">
+      <c r="B57" s="123" t="s">
         <v>347</v>
       </c>
-      <c r="C57" s="122"/>
+      <c r="C57" s="123"/>
     </row>
     <row r="58" spans="1:3" ht="33" customHeight="1">
-      <c r="B58" s="122" t="s">
+      <c r="B58" s="123" t="s">
         <v>348</v>
       </c>
-      <c r="C58" s="122"/>
+      <c r="C58" s="123"/>
     </row>
     <row r="59" spans="1:3" ht="19.5" customHeight="1">
-      <c r="B59" s="122" t="s">
+      <c r="B59" s="123" t="s">
         <v>349</v>
       </c>
-      <c r="C59" s="122"/>
+      <c r="C59" s="123"/>
     </row>
     <row r="60" spans="1:3">
       <c r="B60" s="2" t="s">
@@ -17242,10 +18560,10 @@
       <c r="C87" s="76"/>
     </row>
     <row r="88" spans="1:3" ht="51" customHeight="1">
-      <c r="B88" s="122" t="s">
+      <c r="B88" s="123" t="s">
         <v>400</v>
       </c>
-      <c r="C88" s="122"/>
+      <c r="C88" s="123"/>
     </row>
     <row r="89" spans="1:3" ht="31.5">
       <c r="B89" s="22" t="s">
@@ -17256,13 +18574,13 @@
       <c r="A90" t="s">
         <v>402</v>
       </c>
-      <c r="B90" s="122" t="s">
+      <c r="B90" s="123" t="s">
         <v>401</v>
       </c>
-      <c r="C90" s="122"/>
+      <c r="C90" s="123"/>
     </row>
     <row r="91" spans="1:3" ht="45.75" customHeight="1">
-      <c r="A91" s="123" t="s">
+      <c r="A91" s="124" t="s">
         <v>405</v>
       </c>
       <c r="B91" s="2" t="s">
@@ -17273,7 +18591,7 @@
       </c>
     </row>
     <row r="92" spans="1:3" ht="30">
-      <c r="A92" s="123"/>
+      <c r="A92" s="124"/>
       <c r="B92" s="2" t="s">
         <v>408</v>
       </c>
@@ -17374,8 +18692,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B2:C131"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A114" workbookViewId="0">
-      <selection activeCell="B132" sqref="B132"/>
+    <sheetView topLeftCell="A23" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:C32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -17582,16 +18900,16 @@
       <c r="C26" s="37"/>
     </row>
     <row r="27" spans="2:3" ht="33" customHeight="1">
-      <c r="B27" s="124" t="s">
+      <c r="B27" s="125" t="s">
         <v>294</v>
       </c>
-      <c r="C27" s="124"/>
+      <c r="C27" s="125"/>
     </row>
     <row r="28" spans="2:3">
-      <c r="B28" s="124" t="s">
+      <c r="B28" s="125" t="s">
         <v>295</v>
       </c>
-      <c r="C28" s="124"/>
+      <c r="C28" s="125"/>
     </row>
     <row r="29" spans="2:3" ht="15.75" thickBot="1">
       <c r="B29" s="48" t="s">
@@ -17646,16 +18964,16 @@
       <c r="C37" s="51"/>
     </row>
     <row r="38" spans="2:3" ht="50.25" customHeight="1">
-      <c r="B38" s="124" t="s">
+      <c r="B38" s="125" t="s">
         <v>303</v>
       </c>
-      <c r="C38" s="124"/>
+      <c r="C38" s="125"/>
     </row>
     <row r="39" spans="2:3" ht="32.25" customHeight="1">
-      <c r="B39" s="124" t="s">
+      <c r="B39" s="125" t="s">
         <v>304</v>
       </c>
-      <c r="C39" s="124"/>
+      <c r="C39" s="125"/>
     </row>
     <row r="40" spans="2:3" ht="15.75" thickBot="1">
       <c r="B40" s="52" t="s">
@@ -17705,16 +19023,16 @@
       </c>
     </row>
     <row r="49" spans="2:3" ht="36" customHeight="1">
-      <c r="B49" s="124" t="s">
+      <c r="B49" s="125" t="s">
         <v>314</v>
       </c>
-      <c r="C49" s="124"/>
+      <c r="C49" s="125"/>
     </row>
     <row r="50" spans="2:3" ht="49.5" customHeight="1">
-      <c r="B50" s="124" t="s">
+      <c r="B50" s="125" t="s">
         <v>315</v>
       </c>
-      <c r="C50" s="124"/>
+      <c r="C50" s="125"/>
     </row>
     <row r="52" spans="2:3" ht="41.25">
       <c r="B52" s="91" t="s">
@@ -18200,7 +19518,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B2:C36"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
+    <sheetView topLeftCell="A4" workbookViewId="0">
       <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
@@ -18390,7 +19708,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B2:C131"/>
   <sheetViews>
-    <sheetView topLeftCell="A65" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C39" sqref="C39"/>
     </sheetView>
   </sheetViews>
@@ -19055,4 +20373,471 @@
   <pageSetup orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="B2:C125"/>
+  <sheetViews>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="C16" sqref="C16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="5.140625" customWidth="1"/>
+    <col min="2" max="2" width="54.85546875" customWidth="1"/>
+    <col min="3" max="3" width="107.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:3">
+      <c r="B2" s="38" t="s">
+        <v>46</v>
+      </c>
+      <c r="C2" s="38" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="3" spans="2:3" ht="30.75">
+      <c r="B3" s="128" t="s">
+        <v>627</v>
+      </c>
+      <c r="C3" s="39" t="s">
+        <v>628</v>
+      </c>
+    </row>
+    <row r="4" spans="2:3" ht="45">
+      <c r="B4" s="128" t="s">
+        <v>629</v>
+      </c>
+      <c r="C4" s="39" t="s">
+        <v>630</v>
+      </c>
+    </row>
+    <row r="5" spans="2:3" ht="34.5">
+      <c r="B5" s="129" t="s">
+        <v>631</v>
+      </c>
+      <c r="C5" s="127"/>
+    </row>
+    <row r="6" spans="2:3" ht="19.5" customHeight="1">
+      <c r="B6" s="130" t="s">
+        <v>632</v>
+      </c>
+      <c r="C6" s="2"/>
+    </row>
+    <row r="7" spans="2:3">
+      <c r="B7" s="130" t="s">
+        <v>633</v>
+      </c>
+      <c r="C7" s="115"/>
+    </row>
+    <row r="8" spans="2:3">
+      <c r="B8" s="130" t="s">
+        <v>634</v>
+      </c>
+      <c r="C8" s="2"/>
+    </row>
+    <row r="9" spans="2:3">
+      <c r="B9" s="130" t="s">
+        <v>635</v>
+      </c>
+      <c r="C9" s="2"/>
+    </row>
+    <row r="10" spans="2:3" ht="39">
+      <c r="B10" s="131" t="s">
+        <v>636</v>
+      </c>
+      <c r="C10" s="115" t="s">
+        <v>637</v>
+      </c>
+    </row>
+    <row r="11" spans="2:3" ht="90">
+      <c r="B11" s="132" t="s">
+        <v>640</v>
+      </c>
+      <c r="C11" s="115" t="s">
+        <v>638</v>
+      </c>
+    </row>
+    <row r="12" spans="2:3">
+      <c r="B12" s="132" t="s">
+        <v>639</v>
+      </c>
+      <c r="C12" s="2"/>
+    </row>
+    <row r="13" spans="2:3">
+      <c r="B13" s="132" t="s">
+        <v>641</v>
+      </c>
+      <c r="C13" s="2"/>
+    </row>
+    <row r="14" spans="2:3" ht="125.25">
+      <c r="B14" s="133" t="s">
+        <v>642</v>
+      </c>
+      <c r="C14" s="115" t="s">
+        <v>643</v>
+      </c>
+    </row>
+    <row r="15" spans="2:3" ht="45">
+      <c r="B15" s="131" t="s">
+        <v>644</v>
+      </c>
+      <c r="C15" s="134" t="s">
+        <v>645</v>
+      </c>
+    </row>
+    <row r="16" spans="2:3">
+      <c r="B16" s="4"/>
+      <c r="C16" s="42"/>
+    </row>
+    <row r="17" spans="2:3">
+      <c r="B17" s="2"/>
+      <c r="C17" s="115"/>
+    </row>
+    <row r="18" spans="2:3" ht="18.75" customHeight="1">
+      <c r="B18" s="2"/>
+      <c r="C18" s="40"/>
+    </row>
+    <row r="19" spans="2:3">
+      <c r="B19" s="2"/>
+      <c r="C19" s="115"/>
+    </row>
+    <row r="20" spans="2:3">
+      <c r="B20" s="2"/>
+      <c r="C20" s="115"/>
+    </row>
+    <row r="21" spans="2:3">
+      <c r="B21" s="43"/>
+      <c r="C21" s="40"/>
+    </row>
+    <row r="22" spans="2:3">
+      <c r="B22" s="43"/>
+      <c r="C22" s="40"/>
+    </row>
+    <row r="23" spans="2:3" ht="26.25">
+      <c r="B23" s="44"/>
+      <c r="C23" s="115"/>
+    </row>
+    <row r="24" spans="2:3" ht="33" customHeight="1">
+      <c r="B24" s="125"/>
+      <c r="C24" s="125"/>
+    </row>
+    <row r="25" spans="2:3">
+      <c r="B25" s="125"/>
+      <c r="C25" s="125"/>
+    </row>
+    <row r="26" spans="2:3" ht="15.75" thickBot="1">
+      <c r="B26" s="48"/>
+      <c r="C26" s="49"/>
+    </row>
+    <row r="27" spans="2:3" ht="15.75" thickBot="1">
+      <c r="B27" s="47"/>
+      <c r="C27" s="2"/>
+    </row>
+    <row r="28" spans="2:3" ht="15.75" thickBot="1">
+      <c r="B28" s="46"/>
+      <c r="C28" s="2"/>
+    </row>
+    <row r="29" spans="2:3" ht="15.75" thickBot="1">
+      <c r="B29" s="47"/>
+      <c r="C29" s="2"/>
+    </row>
+    <row r="30" spans="2:3" ht="15.75" thickBot="1">
+      <c r="B30" s="45"/>
+      <c r="C30" s="2"/>
+    </row>
+    <row r="31" spans="2:3" ht="15.75" thickBot="1">
+      <c r="B31" s="47"/>
+      <c r="C31" s="2"/>
+    </row>
+    <row r="32" spans="2:3" ht="15.75" thickBot="1">
+      <c r="B32" s="46"/>
+      <c r="C32" s="2"/>
+    </row>
+    <row r="33" spans="2:3" ht="15.75" thickBot="1">
+      <c r="B33" s="46"/>
+      <c r="C33" s="2"/>
+    </row>
+    <row r="34" spans="2:3">
+      <c r="B34" s="50"/>
+      <c r="C34" s="51"/>
+    </row>
+    <row r="35" spans="2:3" ht="50.25" customHeight="1">
+      <c r="B35" s="125"/>
+      <c r="C35" s="125"/>
+    </row>
+    <row r="36" spans="2:3" ht="32.25" customHeight="1">
+      <c r="B36" s="125"/>
+      <c r="C36" s="125"/>
+    </row>
+    <row r="37" spans="2:3" ht="15.75" thickBot="1">
+      <c r="B37" s="52"/>
+      <c r="C37" s="49"/>
+    </row>
+    <row r="38" spans="2:3" ht="15.75" thickBot="1">
+      <c r="B38" s="46"/>
+      <c r="C38" s="2"/>
+    </row>
+    <row r="39" spans="2:3" ht="15.75" thickBot="1">
+      <c r="B39" s="46"/>
+    </row>
+    <row r="40" spans="2:3" ht="15.75" thickBot="1">
+      <c r="B40" s="46"/>
+    </row>
+    <row r="41" spans="2:3" ht="15.75" thickBot="1">
+      <c r="B41" s="46"/>
+    </row>
+    <row r="42" spans="2:3" ht="15.75" thickBot="1">
+      <c r="B42" s="46"/>
+    </row>
+    <row r="43" spans="2:3" ht="15.75" thickBot="1">
+      <c r="B43" s="46"/>
+    </row>
+    <row r="44" spans="2:3" ht="15.75" thickBot="1">
+      <c r="B44" s="46"/>
+    </row>
+    <row r="45" spans="2:3">
+      <c r="B45" s="50"/>
+    </row>
+    <row r="46" spans="2:3" ht="36" customHeight="1">
+      <c r="B46" s="125"/>
+      <c r="C46" s="125"/>
+    </row>
+    <row r="47" spans="2:3" ht="49.5" customHeight="1">
+      <c r="B47" s="125"/>
+      <c r="C47" s="125"/>
+    </row>
+    <row r="49" spans="2:2" ht="41.25">
+      <c r="B49" s="91"/>
+    </row>
+    <row r="50" spans="2:2">
+      <c r="B50" s="92"/>
+    </row>
+    <row r="51" spans="2:2">
+      <c r="B51" s="93"/>
+    </row>
+    <row r="52" spans="2:2">
+      <c r="B52" s="93"/>
+    </row>
+    <row r="53" spans="2:2">
+      <c r="B53" s="93"/>
+    </row>
+    <row r="54" spans="2:2">
+      <c r="B54" s="94"/>
+    </row>
+    <row r="55" spans="2:2">
+      <c r="B55" s="95"/>
+    </row>
+    <row r="56" spans="2:2">
+      <c r="B56" s="96"/>
+    </row>
+    <row r="57" spans="2:2">
+      <c r="B57" s="96"/>
+    </row>
+    <row r="58" spans="2:2">
+      <c r="B58" s="96"/>
+    </row>
+    <row r="59" spans="2:2">
+      <c r="B59" s="96"/>
+    </row>
+    <row r="60" spans="2:2">
+      <c r="B60" s="95"/>
+    </row>
+    <row r="61" spans="2:2">
+      <c r="B61" s="96"/>
+    </row>
+    <row r="62" spans="2:2">
+      <c r="B62" s="96"/>
+    </row>
+    <row r="63" spans="2:2">
+      <c r="B63" s="96"/>
+    </row>
+    <row r="64" spans="2:2">
+      <c r="B64" s="96"/>
+    </row>
+    <row r="65" spans="2:2">
+      <c r="B65" s="95"/>
+    </row>
+    <row r="66" spans="2:2">
+      <c r="B66" s="96"/>
+    </row>
+    <row r="67" spans="2:2">
+      <c r="B67" s="96"/>
+    </row>
+    <row r="68" spans="2:2">
+      <c r="B68" s="96"/>
+    </row>
+    <row r="69" spans="2:2">
+      <c r="B69" s="96"/>
+    </row>
+    <row r="70" spans="2:2">
+      <c r="B70" s="96"/>
+    </row>
+    <row r="71" spans="2:2">
+      <c r="B71" s="96"/>
+    </row>
+    <row r="72" spans="2:2">
+      <c r="B72" s="96"/>
+    </row>
+    <row r="73" spans="2:2">
+      <c r="B73" s="95"/>
+    </row>
+    <row r="74" spans="2:2">
+      <c r="B74" s="96"/>
+    </row>
+    <row r="75" spans="2:2">
+      <c r="B75" s="96"/>
+    </row>
+    <row r="76" spans="2:2">
+      <c r="B76" s="96"/>
+    </row>
+    <row r="77" spans="2:2">
+      <c r="B77" s="96"/>
+    </row>
+    <row r="78" spans="2:2">
+      <c r="B78" s="95"/>
+    </row>
+    <row r="79" spans="2:2">
+      <c r="B79" s="96"/>
+    </row>
+    <row r="80" spans="2:2">
+      <c r="B80" s="96"/>
+    </row>
+    <row r="81" spans="2:2">
+      <c r="B81" s="96"/>
+    </row>
+    <row r="82" spans="2:2">
+      <c r="B82" s="96"/>
+    </row>
+    <row r="83" spans="2:2">
+      <c r="B83" s="96"/>
+    </row>
+    <row r="84" spans="2:2">
+      <c r="B84" s="96"/>
+    </row>
+    <row r="85" spans="2:2">
+      <c r="B85" s="96"/>
+    </row>
+    <row r="86" spans="2:2">
+      <c r="B86" s="95"/>
+    </row>
+    <row r="87" spans="2:2">
+      <c r="B87" s="97"/>
+    </row>
+    <row r="88" spans="2:2">
+      <c r="B88" s="92"/>
+    </row>
+    <row r="89" spans="2:2">
+      <c r="B89" s="97"/>
+    </row>
+    <row r="90" spans="2:2">
+      <c r="B90" s="97"/>
+    </row>
+    <row r="91" spans="2:2">
+      <c r="B91" s="97"/>
+    </row>
+    <row r="92" spans="2:2">
+      <c r="B92" s="97"/>
+    </row>
+    <row r="93" spans="2:2">
+      <c r="B93" s="97"/>
+    </row>
+    <row r="97" spans="2:2">
+      <c r="B97" s="97"/>
+    </row>
+    <row r="98" spans="2:2">
+      <c r="B98" s="97"/>
+    </row>
+    <row r="99" spans="2:2">
+      <c r="B99" s="92"/>
+    </row>
+    <row r="100" spans="2:2">
+      <c r="B100" s="98"/>
+    </row>
+    <row r="101" spans="2:2">
+      <c r="B101" s="98"/>
+    </row>
+    <row r="103" spans="2:2">
+      <c r="B103" s="94"/>
+    </row>
+    <row r="104" spans="2:2">
+      <c r="B104" s="95"/>
+    </row>
+    <row r="105" spans="2:2">
+      <c r="B105" s="96"/>
+    </row>
+    <row r="106" spans="2:2">
+      <c r="B106" s="96"/>
+    </row>
+    <row r="107" spans="2:2">
+      <c r="B107" s="96"/>
+    </row>
+    <row r="108" spans="2:2">
+      <c r="B108" s="96"/>
+    </row>
+    <row r="109" spans="2:2">
+      <c r="B109" s="96"/>
+    </row>
+    <row r="110" spans="2:2">
+      <c r="B110" s="95"/>
+    </row>
+    <row r="111" spans="2:2">
+      <c r="B111" s="96"/>
+    </row>
+    <row r="112" spans="2:2">
+      <c r="B112" s="96"/>
+    </row>
+    <row r="113" spans="2:2">
+      <c r="B113" s="95"/>
+    </row>
+    <row r="114" spans="2:2">
+      <c r="B114" s="96"/>
+    </row>
+    <row r="115" spans="2:2">
+      <c r="B115" s="96"/>
+    </row>
+    <row r="116" spans="2:2">
+      <c r="B116" s="96"/>
+    </row>
+    <row r="117" spans="2:2">
+      <c r="B117" s="96"/>
+    </row>
+    <row r="118" spans="2:2">
+      <c r="B118" s="96"/>
+    </row>
+    <row r="119" spans="2:2">
+      <c r="B119" s="96"/>
+    </row>
+    <row r="120" spans="2:2">
+      <c r="B120" s="96"/>
+    </row>
+    <row r="121" spans="2:2">
+      <c r="B121" s="96"/>
+    </row>
+    <row r="122" spans="2:2">
+      <c r="B122" s="96"/>
+    </row>
+    <row r="123" spans="2:2">
+      <c r="B123" s="96"/>
+    </row>
+    <row r="124" spans="2:2">
+      <c r="B124" s="95"/>
+    </row>
+    <row r="125" spans="2:2">
+      <c r="B125" s="96"/>
+    </row>
+  </sheetData>
+  <mergeCells count="6">
+    <mergeCell ref="B24:C24"/>
+    <mergeCell ref="B25:C25"/>
+    <mergeCell ref="B35:C35"/>
+    <mergeCell ref="B36:C36"/>
+    <mergeCell ref="B46:C46"/>
+    <mergeCell ref="B47:C47"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>